<commit_message>
new data, new refs 27.3.
</commit_message>
<xml_diff>
--- a/TI_Lombardia.xlsx
+++ b/TI_Lombardia.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80794191\Documents\githubJupyter\COVID-19\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$E$20</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +27,7 @@
     <author>Steinmann Philipp BAG</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -95,13 +93,25 @@
   </si>
   <si>
     <t>de.wikipedia.org/wiki/COVID-19-Pandemie_in_der_Schweiz</t>
+  </si>
+  <si>
+    <t>pop TI</t>
+  </si>
+  <si>
+    <t>ilmessaggero.it</t>
+  </si>
+  <si>
+    <t>pop Lombardia</t>
+  </si>
+  <si>
+    <t>10.04 mio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +143,12 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="23"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -154,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -170,6 +186,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -450,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -462,11 +479,24 @@
     <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="29.25" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="7">
+        <v>353709</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
       </c>
       <c r="J1" t="s">
         <v>12</v>
@@ -496,18 +526,17 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>43914</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1211</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
-        <v>53</v>
+      <c r="A4" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B4">
+        <v>28761</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>3776</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
@@ -518,353 +547,406 @@
       </c>
       <c r="I4" s="6" t="str">
         <f>MONTH(A4)&amp;"/"&amp;DAY(A4)&amp;"/"&amp;(YEAR(A4)-2000)</f>
-        <v>3/24/20</v>
+        <v>3/23/20</v>
       </c>
       <c r="J4" s="4" t="str">
         <f>D4&amp;$J$1&amp;C4&amp;$J$1&amp;"0"&amp;$J$1&amp;"0"&amp;$J$1&amp;I4&amp;$J$1&amp;B4&amp;$J$1&amp;E4</f>
-        <v>,TI,0,0,3/24/20,1211,53</v>
+        <v>,Lombardia,0,0,3/23/20,28761,3776</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43913</v>
+        <v>43914</v>
       </c>
       <c r="B5">
-        <v>28761</v>
+        <v>32346</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="E5">
-        <v>3776</v>
+        <v>4474</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="6" t="str">
         <f>MONTH(A5)&amp;"/"&amp;DAY(A5)&amp;"/"&amp;(YEAR(A5)-2000)</f>
-        <v>3/23/20</v>
+        <v>3/24/20</v>
       </c>
       <c r="J5" s="4" t="str">
         <f>D5&amp;$J$1&amp;C5&amp;$J$1&amp;"0"&amp;$J$1&amp;"0"&amp;$J$1&amp;I5&amp;$J$1&amp;B5&amp;$J$1&amp;E5</f>
-        <v>,Lombardia,0,0,3/23/20,28761,3776</v>
+        <v>,Lombardia,0,0,3/24/20,32346,4474</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>43914</v>
+        <v>43916</v>
       </c>
       <c r="B6">
-        <v>32346</v>
+        <v>34889</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="E6">
-        <v>4474</v>
+        <v>4861</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="6" t="str">
-        <f t="shared" ref="I6:I10" si="0">MONTH(A6)&amp;"/"&amp;DAY(A6)&amp;"/"&amp;(YEAR(A6)-2000)</f>
-        <v>3/24/20</v>
+        <f t="shared" ref="I6:I11" si="0">MONTH(A6)&amp;"/"&amp;DAY(A6)&amp;"/"&amp;(YEAR(A6)-2000)</f>
+        <v>3/26/20</v>
       </c>
       <c r="J6" s="4" t="str">
-        <f t="shared" ref="J6:J10" si="1">D6&amp;$J$1&amp;C6&amp;$J$1&amp;"0"&amp;$J$1&amp;"0"&amp;$J$1&amp;I6&amp;$J$1&amp;B6&amp;$J$1&amp;E6</f>
-        <v>,Lombardia,0,0,3/24/20,32346,4474</v>
+        <f t="shared" ref="J6:J11" si="1">D6&amp;$J$1&amp;C6&amp;$J$1&amp;"0"&amp;$J$1&amp;"0"&amp;$J$1&amp;I6&amp;$J$1&amp;B6&amp;$J$1&amp;E6</f>
+        <v>,Lombardia,0,0,3/26/20,34889,4861</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43915</v>
+        <v>43917</v>
       </c>
       <c r="B7">
-        <v>1343</v>
+        <v>37298</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E7">
-        <v>60</v>
+        <v>5402</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I7" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>3/25/20</v>
+        <f t="shared" ref="I7" si="2">MONTH(A7)&amp;"/"&amp;DAY(A7)&amp;"/"&amp;(YEAR(A7)-2000)</f>
+        <v>3/27/20</v>
       </c>
       <c r="J7" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>,TI,0,0,3/25/20,1343,60</v>
+        <f t="shared" ref="J7" si="3">D7&amp;$J$1&amp;C7&amp;$J$1&amp;"0"&amp;$J$1&amp;"0"&amp;$J$1&amp;I7&amp;$J$1&amp;B7&amp;$J$1&amp;E7</f>
+        <v>,Lombardia,0,0,3/27/20,37298,5402</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>43916</v>
+        <v>43904</v>
       </c>
       <c r="B8">
-        <v>34889</v>
+        <v>262</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>4861</v>
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
       </c>
       <c r="I8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3/26/20</v>
+        <v>3/14/20</v>
       </c>
       <c r="J8" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>,Lombardia,0,0,3/26/20,34889,4861</v>
+        <v>,TI,0,0,3/14/20,262,5</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>43916</v>
+        <v>43905</v>
       </c>
       <c r="B9">
-        <v>1401</v>
+        <v>291</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="E9">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="I9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3/26/20</v>
+        <v>3/15/20</v>
       </c>
       <c r="J9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>,TI,0,0,3/26/20,1401,67</v>
+        <v>,TI,0,0,3/15/20,291,6</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>43904</v>
+        <v>43906</v>
       </c>
       <c r="B10">
-        <v>262</v>
+        <v>330</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3/14/20</v>
+        <v>3/16/20</v>
       </c>
       <c r="J10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>,TI,0,0,3/14/20,262,5</v>
+        <v>,TI,0,0,3/16/20,330,8</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>43905</v>
+        <v>43907</v>
       </c>
       <c r="B11">
-        <v>291</v>
+        <v>422</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I11" s="6" t="str">
-        <f t="shared" ref="I11:I19" si="2">MONTH(A11)&amp;"/"&amp;DAY(A11)&amp;"/"&amp;(YEAR(A11)-2000)</f>
-        <v>3/15/20</v>
+        <f t="shared" si="0"/>
+        <v>3/17/20</v>
       </c>
       <c r="J11" s="4" t="str">
-        <f t="shared" ref="J11:J19" si="3">D11&amp;$J$1&amp;C11&amp;$J$1&amp;"0"&amp;$J$1&amp;"0"&amp;$J$1&amp;I11&amp;$J$1&amp;B11&amp;$J$1&amp;E11</f>
-        <v>,TI,0,0,3/15/20,291,6</v>
+        <f t="shared" si="1"/>
+        <v>,TI,0,0,3/17/20,422,10</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>43906</v>
+        <v>43908</v>
       </c>
       <c r="B12">
-        <v>330</v>
+        <v>511</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="E12">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I12" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>3/16/20</v>
+        <f t="shared" ref="I12:I20" si="4">MONTH(A12)&amp;"/"&amp;DAY(A12)&amp;"/"&amp;(YEAR(A12)-2000)</f>
+        <v>3/18/20</v>
       </c>
       <c r="J12" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>,TI,0,0,3/16/20,330,8</v>
+        <f t="shared" ref="J12:J20" si="5">D12&amp;$J$1&amp;C12&amp;$J$1&amp;"0"&amp;$J$1&amp;"0"&amp;$J$1&amp;I12&amp;$J$1&amp;B12&amp;$J$1&amp;E12</f>
+        <v>,TI,0,0,3/18/20,511,14</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>43907</v>
+        <v>43909</v>
       </c>
       <c r="B13">
-        <v>422</v>
+        <v>638</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I13" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>3/17/20</v>
+        <f t="shared" si="4"/>
+        <v>3/19/20</v>
       </c>
       <c r="J13" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>,TI,0,0,3/17/20,422,10</v>
+        <f t="shared" si="5"/>
+        <v>,TI,0,0,3/19/20,638,15</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>43908</v>
+        <v>43910</v>
       </c>
       <c r="B14">
-        <v>511</v>
+        <v>834</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="E14">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I14" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>3/18/20</v>
+        <f t="shared" si="4"/>
+        <v>3/20/20</v>
       </c>
       <c r="J14" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>,TI,0,0,3/18/20,511,14</v>
+        <f t="shared" si="5"/>
+        <v>,TI,0,0,3/20/20,834,22</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>43909</v>
+        <v>43911</v>
       </c>
       <c r="B15">
-        <v>638</v>
+        <v>918</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I15" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>3/19/20</v>
+        <f t="shared" si="4"/>
+        <v>3/21/20</v>
       </c>
       <c r="J15" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>,TI,0,0,3/19/20,638,15</v>
+        <f t="shared" si="5"/>
+        <v>,TI,0,0,3/21/20,918,28</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>43910</v>
+        <v>43912</v>
       </c>
       <c r="B16">
-        <v>834</v>
+        <v>939</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="E16">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="I16" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>3/20/20</v>
+        <f t="shared" si="4"/>
+        <v>3/22/20</v>
       </c>
       <c r="J16" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>,TI,0,0,3/20/20,834,22</v>
+        <f t="shared" si="5"/>
+        <v>,TI,0,0,3/22/20,939,37</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>43911</v>
+        <v>43913</v>
       </c>
       <c r="B17">
-        <v>918</v>
+        <v>1165</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="E17">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="I17" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>3/21/20</v>
+        <f t="shared" si="4"/>
+        <v>3/23/20</v>
       </c>
       <c r="J17" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>,TI,0,0,3/21/20,918,28</v>
+        <f t="shared" si="5"/>
+        <v>,TI,0,0,3/23/20,1165,48</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>43912</v>
+      <c r="A18" s="2">
+        <v>43914</v>
       </c>
       <c r="B18">
-        <v>939</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
+        <v>1211</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="E18">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="I18" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>3/22/20</v>
+        <f t="shared" si="4"/>
+        <v>3/24/20</v>
       </c>
       <c r="J18" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>,TI,0,0,3/22/20,939,37</v>
+        <f t="shared" si="5"/>
+        <v>,TI,0,0,3/24/20,1211,53</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>43913</v>
+        <v>43915</v>
       </c>
       <c r="B19">
-        <v>1165</v>
+        <v>1343</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="E19">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="I19" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>3/23/20</v>
+        <f t="shared" si="4"/>
+        <v>3/25/20</v>
       </c>
       <c r="J19" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>,TI,0,0,3/23/20,1165,48</v>
+        <f t="shared" si="5"/>
+        <v>,TI,0,0,3/25/20,1343,60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43916</v>
+      </c>
+      <c r="B20">
+        <v>1401</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>67</v>
+      </c>
+      <c r="I20" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>3/26/20</v>
+      </c>
+      <c r="J20" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>,TI,0,0,3/26/20,1401,67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B21">
+        <v>1688</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>76</v>
+      </c>
+      <c r="I21" s="6" t="str">
+        <f t="shared" ref="I21" si="6">MONTH(A21)&amp;"/"&amp;DAY(A21)&amp;"/"&amp;(YEAR(A21)-2000)</f>
+        <v>3/27/20</v>
+      </c>
+      <c r="J21" s="4" t="str">
+        <f t="shared" ref="J21" si="7">D21&amp;$J$1&amp;C21&amp;$J$1&amp;"0"&amp;$J$1&amp;"0"&amp;$J$1&amp;I21&amp;$J$1&amp;B21&amp;$J$1&amp;E21</f>
+        <v>,TI,0,0,3/27/20,1688,76</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:E20">
+    <sortState ref="A4:E20">
+      <sortCondition ref="C3:C19"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
11 countries, 2 figs BFS
</commit_message>
<xml_diff>
--- a/TI_Lombardia.xlsx
+++ b/TI_Lombardia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TI Lombardia" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cases!$A$3:$AB$44</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TI Lombardia'!$A$3:$F$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TI Lombardia'!$A$3:$F$50</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="117">
   <si>
     <t>Date</t>
   </si>
@@ -739,7 +739,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -874,6 +874,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -929,7 +935,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1015,6 +1021,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1023,7 +1040,7 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1157,6 +1174,12 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2872,10 +2895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U60"/>
+  <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L64" sqref="L4:L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3988,900 +4011,1036 @@
         <v>6/4/2020,6,4,2020,1079,297,Lombardia,nn,nnn,10040001</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>43901</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>68</v>
+        <v>43928</v>
+      </c>
+      <c r="B34" s="57">
+        <v>9484</v>
+      </c>
+      <c r="C34" s="57">
+        <v>52325</v>
       </c>
       <c r="D34">
-        <f>C34</f>
-        <v>68</v>
+        <f t="shared" ref="D34" si="7">C34-C33</f>
+        <v>791</v>
       </c>
       <c r="E34" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="G34">
-        <f t="shared" ref="G34:G36" si="7">B34</f>
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <v>353709</v>
+        <f t="shared" ref="G34" si="8">B34-B33</f>
+        <v>282</v>
+      </c>
+      <c r="H34" s="2">
+        <v>10040002</v>
       </c>
       <c r="K34" s="5" t="str">
-        <f t="shared" ref="K34:K36" si="8">DAY(A34)&amp;"/"&amp;MONTH(A34)&amp;"/"&amp;YEAR(A34)</f>
-        <v>11/3/2020</v>
+        <f t="shared" ref="K34" si="9">DAY(A34)&amp;"/"&amp;MONTH(A34)&amp;"/"&amp;YEAR(A34)</f>
+        <v>7/4/2020</v>
       </c>
       <c r="L34" s="3" t="str">
-        <f t="shared" ref="L34:L36" si="9">K34&amp;$L$1&amp;DAY(A34)&amp;$L$1&amp;MONTH(A34)&amp;$L$1&amp;YEAR(A34)&amp;$L$1&amp;D34&amp;$L$1&amp;G34&amp;$L$1&amp;E34&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H34</f>
-        <v>11/3/2020,11,3,2020,68,1,Ticino,nn,nnn,353709</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+        <f t="shared" ref="L34" si="10">K34&amp;$L$1&amp;DAY(A34)&amp;$L$1&amp;MONTH(A34)&amp;$L$1&amp;YEAR(A34)&amp;$L$1&amp;D34&amp;$L$1&amp;G34&amp;$L$1&amp;E34&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H34</f>
+        <v>7/4/2020,7,4,2020,791,282,Lombardia,nn,nnn,10040002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>43902</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="43">
-        <v>180</v>
+        <v>43929</v>
+      </c>
+      <c r="B35" s="57">
+        <v>9722</v>
+      </c>
+      <c r="C35" s="57">
+        <v>53414</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:D60" si="10">C35-C34</f>
-        <v>112</v>
+        <f t="shared" ref="D35" si="11">C35-C34</f>
+        <v>1089</v>
       </c>
       <c r="E35" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="G35">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>353709</v>
+        <f t="shared" ref="G35" si="12">B35-B34</f>
+        <v>238</v>
+      </c>
+      <c r="H35" s="2">
+        <v>10040003</v>
       </c>
       <c r="K35" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>12/3/2020</v>
+        <f t="shared" ref="K35" si="13">DAY(A35)&amp;"/"&amp;MONTH(A35)&amp;"/"&amp;YEAR(A35)</f>
+        <v>8/4/2020</v>
       </c>
       <c r="L35" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v>12/3/2020,12,3,2020,112,1,Ticino,nn,nnn,353709</v>
+        <f t="shared" ref="L35" si="14">K35&amp;$L$1&amp;DAY(A35)&amp;$L$1&amp;MONTH(A35)&amp;$L$1&amp;YEAR(A35)&amp;$L$1&amp;D35&amp;$L$1&amp;G35&amp;$L$1&amp;E35&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H35</f>
+        <v>8/4/2020,8,4,2020,1089,238,Lombardia,nn,nnn,10040003</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>43903</v>
+        <v>43901</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36" s="43">
-        <v>258</v>
+      <c r="C36">
+        <v>68</v>
       </c>
       <c r="D36">
-        <f t="shared" si="10"/>
-        <v>78</v>
+        <f>C36</f>
+        <v>68</v>
       </c>
       <c r="E36" t="s">
         <v>116</v>
       </c>
       <c r="G36">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="G36:G38" si="15">B36</f>
         <v>1</v>
       </c>
       <c r="H36">
         <v>353709</v>
       </c>
       <c r="K36" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>13/3/2020</v>
+        <f t="shared" ref="K36:K38" si="16">DAY(A36)&amp;"/"&amp;MONTH(A36)&amp;"/"&amp;YEAR(A36)</f>
+        <v>11/3/2020</v>
       </c>
       <c r="L36" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v>13/3/2020,13,3,2020,78,1,Ticino,nn,nnn,353709</v>
+        <f t="shared" ref="L36:L38" si="17">K36&amp;$L$1&amp;DAY(A36)&amp;$L$1&amp;MONTH(A36)&amp;$L$1&amp;YEAR(A36)&amp;$L$1&amp;D36&amp;$L$1&amp;G36&amp;$L$1&amp;E36&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H36</f>
+        <v>11/3/2020,11,3,2020,68,1,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>43904</v>
+        <v>43902</v>
       </c>
       <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <v>262</v>
+        <v>1</v>
+      </c>
+      <c r="C37" s="43">
+        <v>180</v>
       </c>
       <c r="D37">
-        <f t="shared" si="10"/>
-        <v>4</v>
+        <f t="shared" ref="D37:D62" si="18">C37-C36</f>
+        <v>112</v>
       </c>
       <c r="E37" t="s">
         <v>116</v>
       </c>
       <c r="G37">
-        <f>B37</f>
-        <v>5</v>
+        <f t="shared" si="15"/>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>353709</v>
       </c>
       <c r="K37" s="5" t="str">
-        <f t="shared" ref="K37:K59" si="11">DAY(A37)&amp;"/"&amp;MONTH(A37)&amp;"/"&amp;YEAR(A37)</f>
-        <v>14/3/2020</v>
+        <f t="shared" si="16"/>
+        <v>12/3/2020</v>
       </c>
       <c r="L37" s="3" t="str">
-        <f t="shared" ref="L37:L59" si="12">K37&amp;$L$1&amp;DAY(A37)&amp;$L$1&amp;MONTH(A37)&amp;$L$1&amp;YEAR(A37)&amp;$L$1&amp;D37&amp;$L$1&amp;G37&amp;$L$1&amp;E37&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H37</f>
-        <v>14/3/2020,14,3,2020,4,5,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="17"/>
+        <v>12/3/2020,12,3,2020,112,1,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>43905</v>
+        <v>43903</v>
       </c>
       <c r="B38">
-        <v>6</v>
-      </c>
-      <c r="C38">
-        <v>291</v>
+        <v>1</v>
+      </c>
+      <c r="C38" s="43">
+        <v>258</v>
       </c>
       <c r="D38">
-        <f t="shared" si="10"/>
-        <v>29</v>
+        <f t="shared" si="18"/>
+        <v>78</v>
       </c>
       <c r="E38" t="s">
         <v>116</v>
       </c>
       <c r="G38">
-        <f t="shared" ref="G38:G59" si="13">B38-B37</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="H38">
         <v>353709</v>
       </c>
       <c r="K38" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>15/3/2020</v>
+        <f t="shared" si="16"/>
+        <v>13/3/2020</v>
       </c>
       <c r="L38" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>15/3/2020,15,3,2020,29,1,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="17"/>
+        <v>13/3/2020,13,3,2020,78,1,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43906</v>
+        <v>43904</v>
       </c>
       <c r="B39">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C39">
-        <v>330</v>
+        <v>262</v>
       </c>
       <c r="D39">
-        <f t="shared" si="10"/>
-        <v>39</v>
+        <f t="shared" si="18"/>
+        <v>4</v>
       </c>
       <c r="E39" t="s">
         <v>116</v>
       </c>
       <c r="G39">
-        <f t="shared" si="13"/>
-        <v>2</v>
+        <f>B39</f>
+        <v>5</v>
       </c>
       <c r="H39">
         <v>353709</v>
       </c>
       <c r="K39" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>16/3/2020</v>
+        <f t="shared" ref="K39:K61" si="19">DAY(A39)&amp;"/"&amp;MONTH(A39)&amp;"/"&amp;YEAR(A39)</f>
+        <v>14/3/2020</v>
       </c>
       <c r="L39" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>16/3/2020,16,3,2020,39,2,Ticino,nn,nnn,353709</v>
+        <f t="shared" ref="L39:L60" si="20">K39&amp;$L$1&amp;DAY(A39)&amp;$L$1&amp;MONTH(A39)&amp;$L$1&amp;YEAR(A39)&amp;$L$1&amp;D39&amp;$L$1&amp;G39&amp;$L$1&amp;E39&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H39</f>
+        <v>14/3/2020,14,3,2020,4,5,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43907</v>
+        <v>43905</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C40">
-        <v>422</v>
+        <v>291</v>
       </c>
       <c r="D40">
-        <f t="shared" si="10"/>
-        <v>92</v>
+        <f t="shared" si="18"/>
+        <v>29</v>
       </c>
       <c r="E40" t="s">
         <v>116</v>
       </c>
       <c r="G40">
-        <f t="shared" si="13"/>
-        <v>2</v>
+        <f t="shared" ref="G40:G61" si="21">B40-B39</f>
+        <v>1</v>
       </c>
       <c r="H40">
         <v>353709</v>
       </c>
       <c r="K40" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>17/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>15/3/2020</v>
       </c>
       <c r="L40" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>17/3/2020,17,3,2020,92,2,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>15/3/2020,15,3,2020,29,1,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43908</v>
+        <v>43906</v>
       </c>
       <c r="B41">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C41">
-        <v>511</v>
+        <v>330</v>
       </c>
       <c r="D41">
-        <f t="shared" si="10"/>
-        <v>89</v>
+        <f t="shared" si="18"/>
+        <v>39</v>
       </c>
       <c r="E41" t="s">
         <v>116</v>
       </c>
       <c r="G41">
-        <f t="shared" si="13"/>
-        <v>4</v>
+        <f t="shared" si="21"/>
+        <v>2</v>
       </c>
       <c r="H41">
         <v>353709</v>
       </c>
       <c r="K41" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>18/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>16/3/2020</v>
       </c>
       <c r="L41" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>18/3/2020,18,3,2020,89,4,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>16/3/2020,16,3,2020,39,2,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43909</v>
+        <v>43907</v>
       </c>
       <c r="B42">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C42">
-        <v>638</v>
+        <v>422</v>
       </c>
       <c r="D42">
-        <f t="shared" si="10"/>
-        <v>127</v>
+        <f t="shared" si="18"/>
+        <v>92</v>
       </c>
       <c r="E42" t="s">
         <v>116</v>
       </c>
       <c r="G42">
-        <f t="shared" si="13"/>
-        <v>1</v>
+        <f t="shared" si="21"/>
+        <v>2</v>
       </c>
       <c r="H42">
         <v>353709</v>
       </c>
       <c r="K42" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>19/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>17/3/2020</v>
       </c>
       <c r="L42" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>19/3/2020,19,3,2020,127,1,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>17/3/2020,17,3,2020,92,2,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>43910</v>
+        <v>43908</v>
       </c>
       <c r="B43">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C43">
-        <v>834</v>
+        <v>511</v>
       </c>
       <c r="D43">
-        <f t="shared" si="10"/>
-        <v>196</v>
+        <f t="shared" si="18"/>
+        <v>89</v>
       </c>
       <c r="E43" t="s">
         <v>116</v>
       </c>
       <c r="G43">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="21"/>
+        <v>4</v>
       </c>
       <c r="H43">
         <v>353709</v>
       </c>
       <c r="K43" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>20/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>18/3/2020</v>
       </c>
       <c r="L43" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>20/3/2020,20,3,2020,196,7,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>18/3/2020,18,3,2020,89,4,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>43911</v>
+        <v>43909</v>
       </c>
       <c r="B44">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C44">
-        <v>918</v>
+        <v>638</v>
       </c>
       <c r="D44">
-        <f t="shared" si="10"/>
-        <v>84</v>
+        <f t="shared" si="18"/>
+        <v>127</v>
       </c>
       <c r="E44" t="s">
         <v>116</v>
       </c>
       <c r="G44">
-        <f t="shared" si="13"/>
-        <v>6</v>
+        <f t="shared" si="21"/>
+        <v>1</v>
       </c>
       <c r="H44">
         <v>353709</v>
       </c>
       <c r="K44" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>21/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>19/3/2020</v>
       </c>
       <c r="L44" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>21/3/2020,21,3,2020,84,6,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>19/3/2020,19,3,2020,127,1,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43912</v>
+        <v>43910</v>
       </c>
       <c r="B45">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C45">
-        <v>939</v>
+        <v>834</v>
       </c>
       <c r="D45">
-        <f t="shared" si="10"/>
-        <v>21</v>
+        <f t="shared" si="18"/>
+        <v>196</v>
       </c>
       <c r="E45" t="s">
         <v>116</v>
       </c>
       <c r="G45">
-        <f t="shared" si="13"/>
-        <v>9</v>
+        <f t="shared" si="21"/>
+        <v>7</v>
       </c>
       <c r="H45">
         <v>353709</v>
       </c>
       <c r="K45" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>22/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>20/3/2020</v>
       </c>
       <c r="L45" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>22/3/2020,22,3,2020,21,9,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>20/3/2020,20,3,2020,196,7,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43913</v>
+        <v>43911</v>
       </c>
       <c r="B46">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C46">
-        <v>1165</v>
+        <v>918</v>
       </c>
       <c r="D46">
-        <f t="shared" si="10"/>
-        <v>226</v>
+        <f t="shared" si="18"/>
+        <v>84</v>
       </c>
       <c r="E46" t="s">
         <v>116</v>
       </c>
       <c r="G46">
-        <f t="shared" si="13"/>
-        <v>11</v>
+        <f t="shared" si="21"/>
+        <v>6</v>
       </c>
       <c r="H46">
         <v>353709</v>
       </c>
       <c r="K46" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>23/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>21/3/2020</v>
       </c>
       <c r="L46" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>23/3/2020,23,3,2020,226,11,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>21/3/2020,21,3,2020,84,6,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>43914</v>
+        <v>43912</v>
       </c>
       <c r="B47">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C47">
-        <v>1211</v>
+        <v>939</v>
       </c>
       <c r="D47">
-        <f t="shared" si="10"/>
-        <v>46</v>
+        <f t="shared" si="18"/>
+        <v>21</v>
       </c>
       <c r="E47" t="s">
         <v>116</v>
       </c>
-      <c r="F47" s="2"/>
       <c r="G47">
-        <f t="shared" si="13"/>
-        <v>5</v>
+        <f t="shared" si="21"/>
+        <v>9</v>
       </c>
       <c r="H47">
         <v>353709</v>
       </c>
       <c r="K47" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>24/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>22/3/2020</v>
       </c>
       <c r="L47" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>24/3/2020,24,3,2020,46,5,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>22/3/2020,22,3,2020,21,9,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43915</v>
+        <v>43913</v>
       </c>
       <c r="B48">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C48">
-        <v>1343</v>
+        <v>1165</v>
       </c>
       <c r="D48">
-        <f t="shared" si="10"/>
-        <v>132</v>
+        <f t="shared" si="18"/>
+        <v>226</v>
       </c>
       <c r="E48" t="s">
         <v>116</v>
       </c>
       <c r="G48">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="21"/>
+        <v>11</v>
       </c>
       <c r="H48">
         <v>353709</v>
       </c>
       <c r="K48" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>25/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>23/3/2020</v>
       </c>
       <c r="L48" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>25/3/2020,25,3,2020,132,7,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>23/3/2020,23,3,2020,226,11,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>43916</v>
+        <v>43914</v>
       </c>
       <c r="B49">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C49">
-        <v>1401</v>
+        <v>1211</v>
       </c>
       <c r="D49">
-        <f t="shared" si="10"/>
-        <v>58</v>
+        <f t="shared" si="18"/>
+        <v>46</v>
       </c>
       <c r="E49" t="s">
         <v>116</v>
       </c>
+      <c r="F49" s="2"/>
       <c r="G49">
-        <f t="shared" si="13"/>
-        <v>7</v>
+        <f t="shared" si="21"/>
+        <v>5</v>
       </c>
       <c r="H49">
         <v>353709</v>
       </c>
       <c r="K49" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>26/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>24/3/2020</v>
       </c>
       <c r="L49" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>26/3/2020,26,3,2020,58,7,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>24/3/2020,24,3,2020,46,5,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="B50">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C50">
-        <v>1688</v>
+        <v>1343</v>
       </c>
       <c r="D50">
-        <f t="shared" si="10"/>
-        <v>287</v>
+        <f t="shared" si="18"/>
+        <v>132</v>
       </c>
       <c r="E50" t="s">
         <v>116</v>
       </c>
       <c r="G50">
-        <f t="shared" si="13"/>
-        <v>9</v>
+        <f t="shared" si="21"/>
+        <v>7</v>
       </c>
       <c r="H50">
         <v>353709</v>
       </c>
       <c r="K50" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>27/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>25/3/2020</v>
       </c>
       <c r="L50" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>27/3/2020,27,3,2020,287,9,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>25/3/2020,25,3,2020,132,7,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>43918</v>
+        <v>43916</v>
       </c>
       <c r="B51">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C51">
-        <v>1727</v>
+        <v>1401</v>
       </c>
       <c r="D51">
-        <f t="shared" si="10"/>
-        <v>39</v>
+        <f t="shared" si="18"/>
+        <v>58</v>
       </c>
       <c r="E51" t="s">
         <v>116</v>
       </c>
       <c r="G51">
-        <f t="shared" si="13"/>
-        <v>11</v>
+        <f t="shared" si="21"/>
+        <v>7</v>
       </c>
       <c r="H51">
         <v>353709</v>
       </c>
       <c r="K51" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>28/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>26/3/2020</v>
       </c>
       <c r="L51" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>28/3/2020,28,3,2020,39,11,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>26/3/2020,26,3,2020,58,7,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>43919</v>
+        <v>43917</v>
       </c>
       <c r="B52">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C52">
-        <v>1837</v>
+        <v>1688</v>
       </c>
       <c r="D52">
-        <f t="shared" si="10"/>
-        <v>110</v>
+        <f t="shared" si="18"/>
+        <v>287</v>
       </c>
       <c r="E52" t="s">
         <v>116</v>
       </c>
       <c r="G52">
-        <f t="shared" si="13"/>
-        <v>6</v>
+        <f t="shared" si="21"/>
+        <v>9</v>
       </c>
       <c r="H52">
         <v>353709</v>
       </c>
       <c r="K52" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>29/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>27/3/2020</v>
       </c>
       <c r="L52" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>29/3/2020,29,3,2020,110,6,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>27/3/2020,27,3,2020,287,9,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>43920</v>
+        <v>43918</v>
       </c>
       <c r="B53">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C53">
-        <v>1962</v>
+        <v>1727</v>
       </c>
       <c r="D53">
-        <f t="shared" si="10"/>
-        <v>125</v>
+        <f t="shared" si="18"/>
+        <v>39</v>
       </c>
       <c r="E53" t="s">
         <v>116</v>
       </c>
       <c r="G53">
-        <f t="shared" si="13"/>
-        <v>12</v>
+        <f t="shared" si="21"/>
+        <v>11</v>
       </c>
       <c r="H53">
         <v>353709</v>
       </c>
       <c r="K53" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>30/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>28/3/2020</v>
       </c>
       <c r="L53" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>30/3/2020,30,3,2020,125,12,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>28/3/2020,28,3,2020,39,11,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>43921</v>
+        <v>43919</v>
       </c>
       <c r="B54">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="C54">
-        <v>2091</v>
+        <v>1837</v>
       </c>
       <c r="D54">
-        <f t="shared" si="10"/>
-        <v>129</v>
+        <f t="shared" si="18"/>
+        <v>110</v>
       </c>
       <c r="E54" t="s">
         <v>116</v>
       </c>
       <c r="G54">
-        <f t="shared" si="13"/>
-        <v>15</v>
+        <f t="shared" si="21"/>
+        <v>6</v>
       </c>
       <c r="H54">
         <v>353709</v>
       </c>
       <c r="K54" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>31/3/2020</v>
+        <f t="shared" si="19"/>
+        <v>29/3/2020</v>
       </c>
       <c r="L54" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>31/3/2020,31,3,2020,129,15,Ticino,nn,nnn,353709</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>29/3/2020,29,3,2020,110,6,Ticino,nn,nnn,353709</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>43922</v>
+        <v>43920</v>
       </c>
       <c r="B55">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="C55">
-        <v>2195</v>
+        <v>1962</v>
       </c>
       <c r="D55">
-        <f t="shared" si="10"/>
-        <v>104</v>
+        <f t="shared" si="18"/>
+        <v>125</v>
       </c>
       <c r="E55" t="s">
         <v>116</v>
       </c>
       <c r="G55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>12</v>
       </c>
       <c r="H55">
         <v>353709</v>
       </c>
       <c r="K55" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>1/4/2020</v>
+        <f t="shared" si="19"/>
+        <v>30/3/2020</v>
       </c>
       <c r="L55" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>1/4/2020,1,4,2020,104,12,Ticino,nn,nnn,353709</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="20"/>
+        <v>30/3/2020,30,3,2020,125,12,Ticino,nn,nnn,353709</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>43923</v>
-      </c>
-      <c r="B56" s="49">
-        <v>141</v>
-      </c>
-      <c r="C56" s="44">
-        <v>2271</v>
+        <v>43921</v>
+      </c>
+      <c r="B56">
+        <v>120</v>
+      </c>
+      <c r="C56">
+        <v>2091</v>
       </c>
       <c r="D56">
-        <f t="shared" si="10"/>
-        <v>76</v>
+        <f t="shared" si="18"/>
+        <v>129</v>
       </c>
       <c r="E56" t="s">
         <v>116</v>
       </c>
       <c r="G56">
-        <f t="shared" si="13"/>
-        <v>9</v>
+        <f t="shared" si="21"/>
+        <v>15</v>
       </c>
       <c r="H56">
         <v>353709</v>
       </c>
       <c r="K56" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>2/4/2020</v>
+        <f t="shared" si="19"/>
+        <v>31/3/2020</v>
       </c>
       <c r="L56" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>2/4/2020,2,4,2020,76,9,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>31/3/2020,31,3,2020,129,15,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>43924</v>
-      </c>
-      <c r="B57" s="49">
-        <v>155</v>
-      </c>
-      <c r="C57" s="44">
-        <v>2377</v>
+        <v>43922</v>
+      </c>
+      <c r="B57">
+        <v>132</v>
+      </c>
+      <c r="C57">
+        <v>2195</v>
       </c>
       <c r="D57">
-        <f t="shared" si="10"/>
-        <v>106</v>
+        <f t="shared" si="18"/>
+        <v>104</v>
       </c>
       <c r="E57" t="s">
         <v>116</v>
       </c>
       <c r="G57">
-        <f t="shared" si="13"/>
-        <v>14</v>
+        <f t="shared" si="21"/>
+        <v>12</v>
       </c>
       <c r="H57">
         <v>353709</v>
       </c>
       <c r="K57" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>3/4/2020</v>
+        <f t="shared" si="19"/>
+        <v>1/4/2020</v>
       </c>
       <c r="L57" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>3/4/2020,3,4,2020,106,14,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>1/4/2020,1,4,2020,104,12,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>43925</v>
+        <v>43923</v>
       </c>
       <c r="B58" s="49">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="C58" s="44">
-        <v>2422</v>
+        <v>2271</v>
       </c>
       <c r="D58">
-        <f t="shared" si="10"/>
-        <v>45</v>
+        <f t="shared" si="18"/>
+        <v>76</v>
       </c>
       <c r="E58" t="s">
         <v>116</v>
       </c>
       <c r="G58">
-        <f t="shared" si="13"/>
-        <v>10</v>
+        <f t="shared" si="21"/>
+        <v>9</v>
       </c>
       <c r="H58">
         <v>353709</v>
       </c>
       <c r="K58" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>4/4/2020</v>
+        <f t="shared" si="19"/>
+        <v>2/4/2020</v>
       </c>
       <c r="L58" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>4/4/2020,4,4,2020,45,10,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>2/4/2020,2,4,2020,76,9,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>43926</v>
+        <v>43924</v>
       </c>
       <c r="B59" s="49">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="C59" s="44">
-        <v>2508</v>
+        <v>2377</v>
       </c>
       <c r="D59">
-        <f t="shared" si="10"/>
-        <v>86</v>
+        <f t="shared" si="18"/>
+        <v>106</v>
       </c>
       <c r="E59" t="s">
         <v>116</v>
       </c>
       <c r="G59">
-        <f t="shared" si="13"/>
-        <v>12</v>
+        <f t="shared" si="21"/>
+        <v>14</v>
       </c>
       <c r="H59">
         <v>353709</v>
       </c>
       <c r="K59" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>5/4/2020</v>
+        <f t="shared" si="19"/>
+        <v>3/4/2020</v>
       </c>
       <c r="L59" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>5/4/2020,5,4,2020,86,12,Ticino,nn,nnn,353709</v>
+        <f t="shared" si="20"/>
+        <v>3/4/2020,3,4,2020,106,14,Ticino,nn,nnn,353709</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>43927</v>
-      </c>
-      <c r="B60" s="47">
-        <v>189</v>
+        <v>43925</v>
+      </c>
+      <c r="B60" s="49">
+        <v>165</v>
       </c>
       <c r="C60" s="44">
-        <v>2546</v>
+        <v>2422</v>
       </c>
       <c r="D60">
-        <f t="shared" si="10"/>
-        <v>38</v>
+        <f t="shared" si="18"/>
+        <v>45</v>
       </c>
       <c r="E60" t="s">
         <v>116</v>
       </c>
       <c r="G60">
-        <f t="shared" ref="G60" si="14">B60-B59</f>
+        <f t="shared" si="21"/>
+        <v>10</v>
+      </c>
+      <c r="H60">
+        <v>353709</v>
+      </c>
+      <c r="K60" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>4/4/2020</v>
+      </c>
+      <c r="L60" s="3" t="str">
+        <f t="shared" si="20"/>
+        <v>4/4/2020,4,4,2020,45,10,Ticino,nn,nnn,353709</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43926</v>
+      </c>
+      <c r="B61" s="49">
+        <v>177</v>
+      </c>
+      <c r="C61" s="44">
+        <v>2508</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="18"/>
+        <v>86</v>
+      </c>
+      <c r="E61" t="s">
+        <v>116</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="H60">
+      <c r="H61">
+        <v>353709</v>
+      </c>
+      <c r="K61" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>5/4/2020</v>
+      </c>
+      <c r="L61" s="3" t="str">
+        <f>K61&amp;$L$1&amp;DAY(A61)&amp;$L$1&amp;MONTH(A61)&amp;$L$1&amp;YEAR(A61)&amp;$L$1&amp;D61&amp;$L$1&amp;G61&amp;$L$1&amp;E61&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H61</f>
+        <v>5/4/2020,5,4,2020,86,12,Ticino,nn,nnn,353709</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B62" s="47">
+        <v>189</v>
+      </c>
+      <c r="C62" s="44">
+        <v>2546</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="18"/>
+        <v>38</v>
+      </c>
+      <c r="E62" t="s">
+        <v>116</v>
+      </c>
+      <c r="G62">
+        <f t="shared" ref="G62:G63" si="22">B62-B61</f>
+        <v>12</v>
+      </c>
+      <c r="H62">
+        <v>353709</v>
+      </c>
+      <c r="K62" s="5" t="str">
+        <f t="shared" ref="K62" si="23">DAY(A62)&amp;"/"&amp;MONTH(A62)&amp;"/"&amp;YEAR(A62)</f>
+        <v>6/4/2020</v>
+      </c>
+      <c r="L62" s="3" t="str">
+        <f t="shared" ref="L62" si="24">K62&amp;$L$1&amp;DAY(A62)&amp;$L$1&amp;MONTH(A62)&amp;$L$1&amp;YEAR(A62)&amp;$L$1&amp;D62&amp;$L$1&amp;G62&amp;$L$1&amp;E62&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H62</f>
+        <v>6/4/2020,6,4,2020,38,12,Ticino,nn,nnn,353709</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B63" s="59">
+        <v>198</v>
+      </c>
+      <c r="C63" s="44">
+        <v>2599</v>
+      </c>
+      <c r="D63">
+        <f t="shared" ref="D63" si="25">C63-C62</f>
+        <v>53</v>
+      </c>
+      <c r="E63" t="s">
+        <v>116</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="22"/>
+        <v>9</v>
+      </c>
+      <c r="H63">
+        <v>353709</v>
+      </c>
+      <c r="K63" s="5" t="str">
+        <f t="shared" ref="K63" si="26">DAY(A63)&amp;"/"&amp;MONTH(A63)&amp;"/"&amp;YEAR(A63)</f>
+        <v>7/4/2020</v>
+      </c>
+      <c r="L63" s="3" t="str">
+        <f t="shared" ref="L63" si="27">K63&amp;$L$1&amp;DAY(A63)&amp;$L$1&amp;MONTH(A63)&amp;$L$1&amp;YEAR(A63)&amp;$L$1&amp;D63&amp;$L$1&amp;G63&amp;$L$1&amp;E63&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H63</f>
+        <v>7/4/2020,7,4,2020,53,9,Ticino,nn,nnn,353709</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B64" s="47">
+        <v>211</v>
+      </c>
+      <c r="C64" s="44">
+        <v>2659</v>
+      </c>
+      <c r="D64">
+        <f t="shared" ref="D64" si="28">C64-C63</f>
+        <v>60</v>
+      </c>
+      <c r="E64" t="s">
+        <v>116</v>
+      </c>
+      <c r="G64">
+        <f t="shared" ref="G64" si="29">B64-B63</f>
+        <v>13</v>
+      </c>
+      <c r="H64">
         <v>353710</v>
       </c>
-      <c r="K60" s="5" t="str">
-        <f t="shared" ref="K60" si="15">DAY(A60)&amp;"/"&amp;MONTH(A60)&amp;"/"&amp;YEAR(A60)</f>
-        <v>6/4/2020</v>
-      </c>
-      <c r="L60" s="3" t="str">
-        <f t="shared" ref="L60" si="16">K60&amp;$L$1&amp;DAY(A60)&amp;$L$1&amp;MONTH(A60)&amp;$L$1&amp;YEAR(A60)&amp;$L$1&amp;D60&amp;$L$1&amp;G60&amp;$L$1&amp;E60&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H60</f>
-        <v>6/4/2020,6,4,2020,38,12,Ticino,nn,nnn,353710</v>
-      </c>
+      <c r="K64" s="5" t="str">
+        <f t="shared" ref="K64" si="30">DAY(A64)&amp;"/"&amp;MONTH(A64)&amp;"/"&amp;YEAR(A64)</f>
+        <v>8/4/2020</v>
+      </c>
+      <c r="L64" s="3" t="str">
+        <f t="shared" ref="L64" si="31">K64&amp;$L$1&amp;DAY(A64)&amp;$L$1&amp;MONTH(A64)&amp;$L$1&amp;YEAR(A64)&amp;$L$1&amp;D64&amp;$L$1&amp;G64&amp;$L$1&amp;E64&amp;$L$1&amp;"nn"&amp;$L$1&amp;"nnn"&amp;$L$1&amp;H64</f>
+        <v>8/4/2020,8,4,2020,60,13,Ticino,nn,nnn,353710</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="57"/>
+      <c r="C65" s="57"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F48">
+  <autoFilter ref="A3:F50">
     <sortState ref="A4:G23">
       <sortCondition ref="E3:E20"/>
     </sortState>
@@ -4894,11 +5053,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD62"/>
+  <dimension ref="A1:BD63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V44" sqref="V44"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AW12" sqref="AW12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9197,7 +9356,7 @@
         <v>19/3/2020,19,3,2020,5024,44,CH,nn,nnn,8543707</v>
       </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39">
         <v>43910</v>
       </c>
@@ -9386,70 +9545,70 @@
       </c>
     </row>
     <row r="28" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39">
+      <c r="A28" s="56">
         <v>43911</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12">
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57">
         <v>418</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="57">
         <v>282</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="57">
         <v>299</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="57">
         <v>167</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I28" s="57">
         <v>1262</v>
       </c>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12">
+      <c r="J28" s="57"/>
+      <c r="K28" s="57">
         <v>239</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="57">
         <v>49</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="57">
         <v>109</v>
       </c>
-      <c r="N28" s="12">
+      <c r="N28" s="57">
         <v>200</v>
       </c>
-      <c r="O28" s="12">
+      <c r="O28" s="57">
         <v>33</v>
       </c>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
-      <c r="S28" s="12"/>
-      <c r="T28" s="12"/>
-      <c r="U28" s="12">
+      <c r="P28" s="57"/>
+      <c r="Q28" s="57"/>
+      <c r="R28" s="57"/>
+      <c r="S28" s="57"/>
+      <c r="T28" s="57"/>
+      <c r="U28" s="57">
         <v>56</v>
       </c>
       <c r="V28" s="44">
         <v>918</v>
       </c>
-      <c r="W28" s="12">
+      <c r="W28" s="57">
         <v>12</v>
       </c>
-      <c r="X28" s="12">
+      <c r="X28" s="57">
         <v>1676</v>
       </c>
-      <c r="Y28" s="12">
+      <c r="Y28" s="57">
         <v>433</v>
       </c>
-      <c r="Z28" s="12"/>
-      <c r="AA28" s="12"/>
-      <c r="AB28" s="12">
+      <c r="Z28" s="57"/>
+      <c r="AA28" s="57"/>
+      <c r="AB28" s="57">
         <v>7368</v>
       </c>
       <c r="AC28" s="15" t="str">
-        <f t="shared" ref="AC28:AC43" si="9">DAY(A28)&amp;"/"&amp;MONTH(A28)&amp;"/"&amp;YEAR(A28)&amp;$AC$1&amp;DAY(A28)&amp;$AC$1&amp;MONTH(A28)&amp;$AC$1&amp;YEAR(A28)</f>
+        <f t="shared" ref="AC28:AC45" si="9">DAY(A28)&amp;"/"&amp;MONTH(A28)&amp;"/"&amp;YEAR(A28)&amp;$AC$1&amp;DAY(A28)&amp;$AC$1&amp;MONTH(A28)&amp;$AC$1&amp;YEAR(A28)</f>
         <v>21/3/2020,21,3,2020</v>
       </c>
       <c r="AD28" s="3" t="str">
@@ -9761,7 +9920,7 @@
         <v>226</v>
       </c>
       <c r="I30" s="57">
-        <v>1509</v>
+        <v>1582</v>
       </c>
       <c r="J30" s="57"/>
       <c r="K30" s="57"/>
@@ -9812,7 +9971,7 @@
         <v>1068</v>
       </c>
       <c r="AB30" s="57">
-        <v>9094</v>
+        <v>9167</v>
       </c>
       <c r="AC30" s="15" t="str">
         <f t="shared" si="9"/>
@@ -9848,7 +10007,7 @@
       </c>
       <c r="AK30" s="3" t="str">
         <f>$AC30&amp;$AC$1&amp;I30&amp;$AC$1&amp;fatalities!I31&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>23/3/2020,23,3,2020,1509,10,GE,nn,nnn,499480</v>
+        <v>23/3/2020,23,3,2020,1582,13,GE,nn,nnn,499480</v>
       </c>
       <c r="AL30" s="3" t="str">
         <f>$AC30&amp;$AC$1&amp;J30&amp;$AC$1&amp;fatalities!J31&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -9924,7 +10083,7 @@
       </c>
       <c r="BD30" s="3" t="str">
         <f>$AC30&amp;$AC$1&amp;AB30&amp;$AC$1&amp;fatalities!AB31&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>23/3/2020,23,3,2020,9094,133,CH,nn,nnn,8543707</v>
+        <v>23/3/2020,23,3,2020,9167,136,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="31" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -9953,7 +10112,7 @@
         <v>255</v>
       </c>
       <c r="I31" s="55">
-        <v>1598</v>
+        <v>1679</v>
       </c>
       <c r="J31" s="55">
         <v>33</v>
@@ -10006,7 +10165,7 @@
         <v>1211</v>
       </c>
       <c r="AB31" s="55">
-        <v>10075</v>
+        <v>10156</v>
       </c>
       <c r="AC31" s="15" t="str">
         <f t="shared" si="9"/>
@@ -10042,7 +10201,7 @@
       </c>
       <c r="AK31" s="3" t="str">
         <f>$AC31&amp;$AC$1&amp;I31&amp;$AC$1&amp;fatalities!I32&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>24/3/2020,24,3,2020,1598,13,GE,nn,nnn,499480</v>
+        <v>24/3/2020,24,3,2020,1679,14,GE,nn,nnn,499480</v>
       </c>
       <c r="AL31" s="3" t="str">
         <f>$AC31&amp;$AC$1&amp;J31&amp;$AC$1&amp;fatalities!J32&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -10118,7 +10277,7 @@
       </c>
       <c r="BD31" s="3" t="str">
         <f>$AC31&amp;$AC$1&amp;AB31&amp;$AC$1&amp;fatalities!AB32&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>24/3/2020,24,3,2020,10075,154,CH,nn,nnn,8543707</v>
+        <v>24/3/2020,24,3,2020,10156,155,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="32" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -10147,7 +10306,7 @@
         <v>293</v>
       </c>
       <c r="I32" s="57">
-        <v>1708</v>
+        <v>1809</v>
       </c>
       <c r="J32" s="57">
         <v>40</v>
@@ -10202,7 +10361,7 @@
         <v>1363</v>
       </c>
       <c r="AB32" s="57">
-        <v>11087</v>
+        <v>11188</v>
       </c>
       <c r="AC32" s="15" t="str">
         <f t="shared" si="9"/>
@@ -10238,7 +10397,7 @@
       </c>
       <c r="AK32" s="3" t="str">
         <f>$AC32&amp;$AC$1&amp;I32&amp;$AC$1&amp;fatalities!I33&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>25/3/2020,25,3,2020,1708,16,GE,nn,nnn,499480</v>
+        <v>25/3/2020,25,3,2020,1809,21,GE,nn,nnn,499480</v>
       </c>
       <c r="AL32" s="3" t="str">
         <f>$AC32&amp;$AC$1&amp;J32&amp;$AC$1&amp;fatalities!J33&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -10314,7 +10473,7 @@
       </c>
       <c r="BD32" s="3" t="str">
         <f>$AC32&amp;$AC$1&amp;AB32&amp;$AC$1&amp;fatalities!AB33&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>25/3/2020,25,3,2020,11087,182,CH,nn,nnn,8543707</v>
+        <v>25/3/2020,25,3,2020,11188,187,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="33" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -10343,7 +10502,7 @@
         <v>309</v>
       </c>
       <c r="I33" s="55">
-        <v>1902</v>
+        <v>2041</v>
       </c>
       <c r="J33" s="55">
         <v>43</v>
@@ -10400,7 +10559,7 @@
         <v>1476</v>
       </c>
       <c r="AB33" s="55">
-        <v>12285</v>
+        <v>12424</v>
       </c>
       <c r="AC33" s="15" t="str">
         <f t="shared" si="9"/>
@@ -10436,7 +10595,7 @@
       </c>
       <c r="AK33" s="3" t="str">
         <f>$AC33&amp;$AC$1&amp;I33&amp;$AC$1&amp;fatalities!I34&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>26/3/2020,26,3,2020,1902,22,GE,nn,nnn,499480</v>
+        <v>26/3/2020,26,3,2020,2041,23,GE,nn,nnn,499480</v>
       </c>
       <c r="AL33" s="3" t="str">
         <f>$AC33&amp;$AC$1&amp;J33&amp;$AC$1&amp;fatalities!J34&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -10512,7 +10671,7 @@
       </c>
       <c r="BD33" s="3" t="str">
         <f>$AC33&amp;$AC$1&amp;AB33&amp;$AC$1&amp;fatalities!AB34&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>26/3/2020,26,3,2020,12285,227,CH,nn,nnn,8543707</v>
+        <v>26/3/2020,26,3,2020,12424,228,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="34" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -10541,7 +10700,7 @@
         <v>369</v>
       </c>
       <c r="I34" s="57">
-        <v>2051</v>
+        <v>2234</v>
       </c>
       <c r="J34" s="57">
         <v>44</v>
@@ -10596,7 +10755,7 @@
         <v>1578</v>
       </c>
       <c r="AB34" s="57">
-        <v>13512</v>
+        <v>13695</v>
       </c>
       <c r="AC34" s="15" t="str">
         <f t="shared" si="9"/>
@@ -10632,7 +10791,7 @@
       </c>
       <c r="AK34" s="3" t="str">
         <f>$AC34&amp;$AC$1&amp;I34&amp;$AC$1&amp;fatalities!I35&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>27/3/2020,27,3,2020,2051,23,GE,nn,nnn,499480</v>
+        <v>27/3/2020,27,3,2020,2234,30,GE,nn,nnn,499480</v>
       </c>
       <c r="AL34" s="3" t="str">
         <f>$AC34&amp;$AC$1&amp;J34&amp;$AC$1&amp;fatalities!J35&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -10708,7 +10867,7 @@
       </c>
       <c r="BD34" s="3" t="str">
         <f>$AC34&amp;$AC$1&amp;AB34&amp;$AC$1&amp;fatalities!AB35&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>27/3/2020,27,3,2020,13512,255,CH,nn,nnn,8543707</v>
+        <v>27/3/2020,27,3,2020,13695,262,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="35" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -10735,7 +10894,7 @@
         <v>421</v>
       </c>
       <c r="I35" s="55">
-        <v>2277</v>
+        <v>2433</v>
       </c>
       <c r="J35" s="55">
         <v>47</v>
@@ -10786,7 +10945,7 @@
         <v>1720</v>
       </c>
       <c r="AB35" s="55">
-        <v>14521</v>
+        <v>14677</v>
       </c>
       <c r="AC35" s="15" t="str">
         <f t="shared" si="9"/>
@@ -10822,7 +10981,7 @@
       </c>
       <c r="AK35" s="3" t="str">
         <f>$AC35&amp;$AC$1&amp;I35&amp;$AC$1&amp;fatalities!I36&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>28/3/2020,28,3,2020,2277,27,GE,nn,nnn,499480</v>
+        <v>28/3/2020,28,3,2020,2433,37,GE,nn,nnn,499480</v>
       </c>
       <c r="AL35" s="3" t="str">
         <f>$AC35&amp;$AC$1&amp;J35&amp;$AC$1&amp;fatalities!J36&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -10898,7 +11057,7 @@
       </c>
       <c r="BD35" s="3" t="str">
         <f>$AC35&amp;$AC$1&amp;AB35&amp;$AC$1&amp;fatalities!AB36&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>28/3/2020,28,3,2020,14521,292,CH,nn,nnn,8543707</v>
+        <v>28/3/2020,28,3,2020,14677,302,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="36" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -10923,7 +11082,7 @@
         <v>442</v>
       </c>
       <c r="I36" s="57">
-        <v>2349</v>
+        <v>2550</v>
       </c>
       <c r="J36" s="57"/>
       <c r="K36" s="57"/>
@@ -10972,7 +11131,7 @@
         <v>1758</v>
       </c>
       <c r="AB36" s="57">
-        <v>15228</v>
+        <v>15429</v>
       </c>
       <c r="AC36" s="15" t="str">
         <f t="shared" si="9"/>
@@ -11008,7 +11167,7 @@
       </c>
       <c r="AK36" s="3" t="str">
         <f>$AC36&amp;$AC$1&amp;I36&amp;$AC$1&amp;fatalities!I37&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>29/3/2020,29,3,2020,2349,37,GE,nn,nnn,499480</v>
+        <v>29/3/2020,29,3,2020,2550,44,GE,nn,nnn,499480</v>
       </c>
       <c r="AL36" s="3" t="str">
         <f>$AC36&amp;$AC$1&amp;J36&amp;$AC$1&amp;fatalities!J37&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -11084,7 +11243,7 @@
       </c>
       <c r="BD36" s="3" t="str">
         <f>$AC36&amp;$AC$1&amp;AB36&amp;$AC$1&amp;fatalities!AB37&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>29/3/2020,29,3,2020,15228,328,CH,nn,nnn,8543707</v>
+        <v>29/3/2020,29,3,2020,15429,335,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="37" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -11113,7 +11272,7 @@
         <v>477</v>
       </c>
       <c r="I37" s="55">
-        <v>2450</v>
+        <v>2764</v>
       </c>
       <c r="J37" s="55">
         <v>50</v>
@@ -11168,7 +11327,7 @@
         <v>1874</v>
       </c>
       <c r="AB37" s="55">
-        <v>16141</v>
+        <v>16455</v>
       </c>
       <c r="AC37" s="15" t="str">
         <f t="shared" si="9"/>
@@ -11204,7 +11363,7 @@
       </c>
       <c r="AK37" s="3" t="str">
         <f>$AC37&amp;$AC$1&amp;I37&amp;$AC$1&amp;fatalities!I38&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>30/3/2020,30,3,2020,2450,43,GE,nn,nnn,499480</v>
+        <v>30/3/2020,30,3,2020,2764,53,GE,nn,nnn,499480</v>
       </c>
       <c r="AL37" s="3" t="str">
         <f>$AC37&amp;$AC$1&amp;J37&amp;$AC$1&amp;fatalities!J38&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -11280,7 +11439,7 @@
       </c>
       <c r="BD37" s="3" t="str">
         <f>$AC37&amp;$AC$1&amp;AB37&amp;$AC$1&amp;fatalities!AB38&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>30/3/2020,30,3,2020,16141,384,CH,nn,nnn,8543707</v>
+        <v>30/3/2020,30,3,2020,16455,394,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="38" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -11309,7 +11468,7 @@
         <v>491</v>
       </c>
       <c r="I38" s="57">
-        <v>2657</v>
+        <v>2994</v>
       </c>
       <c r="J38" s="57">
         <v>53</v>
@@ -11366,7 +11525,7 @@
         <v>1960</v>
       </c>
       <c r="AB38" s="57">
-        <v>17098</v>
+        <v>17435</v>
       </c>
       <c r="AC38" s="15" t="str">
         <f t="shared" si="9"/>
@@ -11402,7 +11561,7 @@
       </c>
       <c r="AK38" s="3" t="str">
         <f>$AC38&amp;$AC$1&amp;I38&amp;$AC$1&amp;fatalities!I39&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>31/3/2020,31,3,2020,2657,52,GE,nn,nnn,499480</v>
+        <v>31/3/2020,31,3,2020,2994,61,GE,nn,nnn,499480</v>
       </c>
       <c r="AL38" s="3" t="str">
         <f>$AC38&amp;$AC$1&amp;J38&amp;$AC$1&amp;fatalities!J39&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -11478,7 +11637,7 @@
       </c>
       <c r="BD38" s="3" t="str">
         <f>$AC38&amp;$AC$1&amp;AB38&amp;$AC$1&amp;fatalities!AB39&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>31/3/2020,31,3,2020,17098,457,CH,nn,nnn,8543707</v>
+        <v>31/3/2020,31,3,2020,17435,466,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="39" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -11505,7 +11664,7 @@
         <v>525</v>
       </c>
       <c r="I39" s="55">
-        <v>2775</v>
+        <v>3161</v>
       </c>
       <c r="J39" s="55">
         <v>56</v>
@@ -11562,7 +11721,7 @@
         <v>2148</v>
       </c>
       <c r="AB39" s="55">
-        <v>18069</v>
+        <v>18455</v>
       </c>
       <c r="AC39" s="15" t="str">
         <f t="shared" si="9"/>
@@ -11598,7 +11757,7 @@
       </c>
       <c r="AK39" s="3" t="str">
         <f>$AC39&amp;$AC$1&amp;I39&amp;$AC$1&amp;fatalities!I40&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>1/4/2020,1,4,2020,2775,65,GE,nn,nnn,499480</v>
+        <v>1/4/2020,1,4,2020,3161,68,GE,nn,nnn,499480</v>
       </c>
       <c r="AL39" s="3" t="str">
         <f>$AC39&amp;$AC$1&amp;J39&amp;$AC$1&amp;fatalities!J40&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -11674,7 +11833,7 @@
       </c>
       <c r="BD39" s="3" t="str">
         <f>$AC39&amp;$AC$1&amp;AB39&amp;$AC$1&amp;fatalities!AB40&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>1/4/2020,1,4,2020,18069,515,CH,nn,nnn,8543707</v>
+        <v>1/4/2020,1,4,2020,18455,518,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="40" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -11703,7 +11862,7 @@
         <v>550</v>
       </c>
       <c r="I40" s="57">
-        <v>2938</v>
+        <v>3369</v>
       </c>
       <c r="J40" s="57">
         <v>58</v>
@@ -11760,7 +11919,7 @@
         <v>2323</v>
       </c>
       <c r="AB40" s="57">
-        <v>19133</v>
+        <v>19564</v>
       </c>
       <c r="AC40" s="15" t="str">
         <f t="shared" si="9"/>
@@ -11796,7 +11955,7 @@
       </c>
       <c r="AK40" s="3" t="str">
         <f>$AC40&amp;$AC$1&amp;I40&amp;$AC$1&amp;fatalities!I41&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>2/4/2020,2,4,2020,2938,72,GE,nn,nnn,499480</v>
+        <v>2/4/2020,2,4,2020,3369,76,GE,nn,nnn,499480</v>
       </c>
       <c r="AL40" s="3" t="str">
         <f>$AC40&amp;$AC$1&amp;J40&amp;$AC$1&amp;fatalities!J41&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -11872,7 +12031,7 @@
       </c>
       <c r="BD40" s="3" t="str">
         <f>$AC40&amp;$AC$1&amp;AB40&amp;$AC$1&amp;fatalities!AB41&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>2/4/2020,2,4,2020,19133,568,CH,nn,nnn,8543707</v>
+        <v>2/4/2020,2,4,2020,19564,572,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="41" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -11901,7 +12060,7 @@
         <v>588</v>
       </c>
       <c r="I41" s="55">
-        <v>3220</v>
+        <v>3561</v>
       </c>
       <c r="J41" s="55">
         <v>59</v>
@@ -11958,7 +12117,7 @@
         <v>2452</v>
       </c>
       <c r="AB41" s="55">
-        <v>20141</v>
+        <v>20482</v>
       </c>
       <c r="AC41" s="15" t="str">
         <f t="shared" si="9"/>
@@ -11994,7 +12153,7 @@
       </c>
       <c r="AK41" s="3" t="str">
         <f>$AC41&amp;$AC$1&amp;I41&amp;$AC$1&amp;fatalities!I42&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>3/4/2020,3,4,2020,3220,78,GE,nn,nnn,499480</v>
+        <v>3/4/2020,3,4,2020,3561,80,GE,nn,nnn,499480</v>
       </c>
       <c r="AL41" s="3" t="str">
         <f>$AC41&amp;$AC$1&amp;J41&amp;$AC$1&amp;fatalities!J42&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -12070,7 +12229,7 @@
       </c>
       <c r="BD41" s="3" t="str">
         <f>$AC41&amp;$AC$1&amp;AB41&amp;$AC$1&amp;fatalities!AB42&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>3/4/2020,3,4,2020,20141,629,CH,nn,nnn,8543707</v>
+        <v>3/4/2020,3,4,2020,20482,631,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="42" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -12097,7 +12256,7 @@
         <v>638</v>
       </c>
       <c r="I42" s="57">
-        <v>3384</v>
+        <v>3683</v>
       </c>
       <c r="J42" s="57"/>
       <c r="K42" s="57"/>
@@ -12107,7 +12266,9 @@
       <c r="M42" s="57">
         <v>469</v>
       </c>
-      <c r="N42" s="57"/>
+      <c r="N42" s="57">
+        <v>449</v>
+      </c>
       <c r="O42" s="57">
         <v>80</v>
       </c>
@@ -12146,7 +12307,7 @@
         <v>2492</v>
       </c>
       <c r="AB42" s="57">
-        <v>20773</v>
+        <v>21088</v>
       </c>
       <c r="AC42" s="15" t="str">
         <f t="shared" si="9"/>
@@ -12182,7 +12343,7 @@
       </c>
       <c r="AK42" s="3" t="str">
         <f>$AC42&amp;$AC$1&amp;I42&amp;$AC$1&amp;fatalities!I43&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>4/4/2020,4,4,2020,3384,83,GE,nn,nnn,499480</v>
+        <v>4/4/2020,4,4,2020,3683,93,GE,nn,nnn,499480</v>
       </c>
       <c r="AL42" s="3" t="str">
         <f>$AC42&amp;$AC$1&amp;J42&amp;$AC$1&amp;fatalities!J43&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -12202,7 +12363,7 @@
       </c>
       <c r="AP42" s="3" t="str">
         <f>$AC42&amp;$AC$1&amp;N42&amp;$AC$1&amp;fatalities!N43&amp;$AC$1&amp;N$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;N$2</f>
-        <v>4/4/2020,4,4,2020,,24,NE,nn,nnn,176850</v>
+        <v>4/4/2020,4,4,2020,449,24,NE,nn,nnn,176850</v>
       </c>
       <c r="AQ42" s="3" t="str">
         <f>$AC42&amp;$AC$1&amp;O42&amp;$AC$1&amp;fatalities!O43&amp;$AC$1&amp;O$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;O$2</f>
@@ -12258,7 +12419,7 @@
       </c>
       <c r="BD42" s="3" t="str">
         <f>$AC42&amp;$AC$1&amp;AB42&amp;$AC$1&amp;fatalities!AB43&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>4/4/2020,4,4,2020,20773,687,CH,nn,nnn,8543707</v>
+        <v>4/4/2020,4,4,2020,21088,697,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="43" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -12283,7 +12444,7 @@
         <v>669</v>
       </c>
       <c r="I43" s="55">
-        <v>3439</v>
+        <v>3750</v>
       </c>
       <c r="J43" s="55"/>
       <c r="K43" s="55">
@@ -12334,7 +12495,7 @@
         <v>2522</v>
       </c>
       <c r="AB43" s="55">
-        <v>21276</v>
+        <v>21587</v>
       </c>
       <c r="AC43" s="15" t="str">
         <f t="shared" si="9"/>
@@ -12370,7 +12531,7 @@
       </c>
       <c r="AK43" s="3" t="str">
         <f>$AC43&amp;$AC$1&amp;I43&amp;$AC$1&amp;fatalities!I44&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>5/4/2020,5,4,2020,3439,92,GE,nn,nnn,499480</v>
+        <v>5/4/2020,5,4,2020,3750,100,GE,nn,nnn,499480</v>
       </c>
       <c r="AL43" s="3" t="str">
         <f>$AC43&amp;$AC$1&amp;J43&amp;$AC$1&amp;fatalities!J44&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -12446,7 +12607,7 @@
       </c>
       <c r="BD43" s="3" t="str">
         <f>$AC43&amp;$AC$1&amp;AB43&amp;$AC$1&amp;fatalities!AB44&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>5/4/2020,5,4,2020,21276,738,CH,nn,nnn,8543707</v>
+        <v>5/4/2020,5,4,2020,21587,746,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="44" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -12471,19 +12632,27 @@
       <c r="G44" s="57">
         <v>803</v>
       </c>
-      <c r="H44" s="57"/>
-      <c r="I44" s="57"/>
+      <c r="H44" s="57">
+        <v>689</v>
+      </c>
+      <c r="I44" s="57">
+        <v>3862</v>
+      </c>
       <c r="J44" s="57">
         <v>63</v>
       </c>
-      <c r="K44" s="57"/>
+      <c r="K44" s="57">
+        <v>657</v>
+      </c>
       <c r="L44" s="57">
         <v>160</v>
       </c>
       <c r="M44" s="57">
         <v>497</v>
       </c>
-      <c r="N44" s="57"/>
+      <c r="N44" s="57">
+        <v>466</v>
+      </c>
       <c r="O44" s="57">
         <v>86</v>
       </c>
@@ -12493,7 +12662,9 @@
       <c r="Q44" s="57">
         <v>532</v>
       </c>
-      <c r="R44" s="57"/>
+      <c r="R44" s="57">
+        <v>50</v>
+      </c>
       <c r="S44" s="57">
         <v>261</v>
       </c>
@@ -12509,7 +12680,9 @@
       <c r="W44" s="57">
         <v>67</v>
       </c>
-      <c r="X44" s="57"/>
+      <c r="X44" s="57">
+        <v>4155</v>
+      </c>
       <c r="Y44" s="57">
         <v>1400</v>
       </c>
@@ -12520,10 +12693,10 @@
         <v>2590</v>
       </c>
       <c r="AB44" s="57">
-        <v>21663</v>
+        <v>22165</v>
       </c>
       <c r="AC44" s="15" t="str">
-        <f t="shared" ref="AC44" si="10">DAY(A44)&amp;"/"&amp;MONTH(A44)&amp;"/"&amp;YEAR(A44)&amp;$AC$1&amp;DAY(A44)&amp;$AC$1&amp;MONTH(A44)&amp;$AC$1&amp;YEAR(A44)</f>
+        <f t="shared" si="9"/>
         <v>6/4/2020,6,4,2020</v>
       </c>
       <c r="AD44" s="3" t="str">
@@ -12552,11 +12725,11 @@
       </c>
       <c r="AJ44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;H44&amp;$AC$1&amp;fatalities!H45&amp;$AC$1&amp;H$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;H$2</f>
-        <v>6/4/2020,6,4,2020,,,FR,nn,nnn,318714</v>
+        <v>6/4/2020,6,4,2020,689,41,FR,nn,nnn,318714</v>
       </c>
       <c r="AK44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;I44&amp;$AC$1&amp;fatalities!I45&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
-        <v>6/4/2020,6,4,2020,,,GE,nn,nnn,499480</v>
+        <v>6/4/2020,6,4,2020,3862,111,GE,nn,nnn,499480</v>
       </c>
       <c r="AL44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;J44&amp;$AC$1&amp;fatalities!J45&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
@@ -12564,7 +12737,7 @@
       </c>
       <c r="AM44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;K44&amp;$AC$1&amp;fatalities!K45&amp;$AC$1&amp;K$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;K$2</f>
-        <v>6/4/2020,6,4,2020,,,GR,nn,nnn,198379</v>
+        <v>6/4/2020,6,4,2020,657,31,GR,nn,nnn,198379</v>
       </c>
       <c r="AN44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;L44&amp;$AC$1&amp;fatalities!L45&amp;$AC$1&amp;L$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;L$2</f>
@@ -12576,7 +12749,7 @@
       </c>
       <c r="AP44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;N44&amp;$AC$1&amp;fatalities!N45&amp;$AC$1&amp;N$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;N$2</f>
-        <v>6/4/2020,6,4,2020,,27,NE,nn,nnn,176850</v>
+        <v>6/4/2020,6,4,2020,466,30,NE,nn,nnn,176850</v>
       </c>
       <c r="AQ44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;O44&amp;$AC$1&amp;fatalities!O45&amp;$AC$1&amp;O$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;O$2</f>
@@ -12592,7 +12765,7 @@
       </c>
       <c r="AT44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;R44&amp;$AC$1&amp;fatalities!R45&amp;$AC$1&amp;R$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;R$2</f>
-        <v>6/4/2020,6,4,2020,,,SH,nn,nnn,81991</v>
+        <v>6/4/2020,6,4,2020,50,1,SH,nn,nnn,81991</v>
       </c>
       <c r="AU44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;S44&amp;$AC$1&amp;fatalities!S45&amp;$AC$1&amp;S$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;S$2</f>
@@ -12616,7 +12789,7 @@
       </c>
       <c r="AZ44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;X44&amp;$AC$1&amp;fatalities!X45&amp;$AC$1&amp;X$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;X$2</f>
-        <v>6/4/2020,6,4,2020,,,VD,nn,nnn,799145</v>
+        <v>6/4/2020,6,4,2020,4155,160,VD,nn,nnn,799145</v>
       </c>
       <c r="BA44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;Y44&amp;$AC$1&amp;fatalities!Y45&amp;$AC$1&amp;Y$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;Y$2</f>
@@ -12632,497 +12805,923 @@
       </c>
       <c r="BD44" s="3" t="str">
         <f>$AC44&amp;$AC$1&amp;AB44&amp;$AC$1&amp;fatalities!AB45&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
-        <v>6/4/2020,6,4,2020,21663,765,CH,nn,nnn,8543707</v>
+        <v>6/4/2020,6,4,2020,22165,802,CH,nn,nnn,8543707</v>
       </c>
     </row>
     <row r="45" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="55"/>
-      <c r="M45" s="55"/>
-      <c r="N45" s="55"/>
-      <c r="O45" s="55"/>
-      <c r="P45" s="55"/>
-      <c r="Q45" s="55"/>
-      <c r="R45" s="55"/>
-      <c r="S45" s="55"/>
-      <c r="T45" s="55"/>
-      <c r="U45" s="55"/>
-      <c r="V45" s="55"/>
-      <c r="W45" s="55"/>
-      <c r="X45" s="55"/>
-      <c r="Y45" s="55"/>
-      <c r="Z45" s="55"/>
-      <c r="AA45" s="55"/>
-      <c r="AB45" s="55"/>
-      <c r="AC45" s="10"/>
+      <c r="A45" s="54">
+        <v>43928</v>
+      </c>
+      <c r="B45" s="55">
+        <v>760</v>
+      </c>
+      <c r="C45" s="55">
+        <v>21</v>
+      </c>
+      <c r="D45" s="55">
+        <v>69</v>
+      </c>
+      <c r="E45" s="55">
+        <v>1228</v>
+      </c>
+      <c r="F45" s="55">
+        <v>690</v>
+      </c>
+      <c r="G45" s="55">
+        <v>813</v>
+      </c>
+      <c r="H45" s="55">
+        <v>729</v>
+      </c>
+      <c r="I45" s="55">
+        <v>3993</v>
+      </c>
+      <c r="J45" s="55">
+        <v>63</v>
+      </c>
+      <c r="K45" s="55">
+        <v>668</v>
+      </c>
+      <c r="L45" s="55">
+        <v>168</v>
+      </c>
+      <c r="M45" s="55">
+        <v>509</v>
+      </c>
+      <c r="N45" s="55">
+        <v>492</v>
+      </c>
+      <c r="O45" s="55">
+        <v>87</v>
+      </c>
+      <c r="P45" s="55">
+        <v>60</v>
+      </c>
+      <c r="Q45" s="55">
+        <v>557</v>
+      </c>
+      <c r="R45" s="55">
+        <v>50</v>
+      </c>
+      <c r="S45" s="55">
+        <v>264</v>
+      </c>
+      <c r="T45" s="55">
+        <v>185</v>
+      </c>
+      <c r="U45" s="55">
+        <v>221</v>
+      </c>
+      <c r="V45" s="44">
+        <v>2599</v>
+      </c>
+      <c r="W45" s="55">
+        <v>68</v>
+      </c>
+      <c r="X45" s="55">
+        <v>4235</v>
+      </c>
+      <c r="Y45" s="55">
+        <v>1436</v>
+      </c>
+      <c r="Z45" s="55">
+        <v>157</v>
+      </c>
+      <c r="AA45" s="55">
+        <v>2719</v>
+      </c>
+      <c r="AB45" s="55">
+        <v>22841</v>
+      </c>
+      <c r="AC45" s="15" t="str">
+        <f t="shared" si="9"/>
+        <v>7/4/2020,7,4,2020</v>
+      </c>
+      <c r="AD45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;B45&amp;$AC$1&amp;fatalities!B46&amp;$AC$1&amp;B$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;B$2</f>
+        <v>7/4/2020,7,4,2020,760,16,AG,nn,nnn,677387</v>
+      </c>
+      <c r="AE45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;C45&amp;$AC$1&amp;fatalities!C46&amp;$AC$1&amp;C$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;C$2</f>
+        <v>7/4/2020,7,4,2020,21,,AI,nn,nnn,16145</v>
+      </c>
+      <c r="AF45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;D45&amp;$AC$1&amp;fatalities!D46&amp;$AC$1&amp;D$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;D$2</f>
+        <v>7/4/2020,7,4,2020,69,3,AR,nn,nnn,55234</v>
+      </c>
+      <c r="AG45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;E45&amp;$AC$1&amp;fatalities!E46&amp;$AC$1&amp;E$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;E$2</f>
+        <v>7/4/2020,7,4,2020,1228,33,BE,nn,nnn,1034977</v>
+      </c>
+      <c r="AH45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;F45&amp;$AC$1&amp;fatalities!F46&amp;$AC$1&amp;F$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;F$2</f>
+        <v>7/4/2020,7,4,2020,690,19,BL,nn,nnn,288132</v>
+      </c>
+      <c r="AI45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;G45&amp;$AC$1&amp;fatalities!G46&amp;$AC$1&amp;G$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;G$2</f>
+        <v>7/4/2020,7,4,2020,813,28,BS,nn,nnn,194766</v>
+      </c>
+      <c r="AJ45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;H45&amp;$AC$1&amp;fatalities!H46&amp;$AC$1&amp;H$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;H$2</f>
+        <v>7/4/2020,7,4,2020,729,44,FR,nn,nnn,318714</v>
+      </c>
+      <c r="AK45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;I45&amp;$AC$1&amp;fatalities!I46&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
+        <v>7/4/2020,7,4,2020,3993,118,GE,nn,nnn,499480</v>
+      </c>
+      <c r="AL45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;J45&amp;$AC$1&amp;fatalities!J46&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
+        <v>7/4/2020,7,4,2020,63,2,GL,nn,nnn,40403</v>
+      </c>
+      <c r="AM45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;K45&amp;$AC$1&amp;fatalities!K46&amp;$AC$1&amp;K$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;K$2</f>
+        <v>7/4/2020,7,4,2020,668,34,GR,nn,nnn,198379</v>
+      </c>
+      <c r="AN45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;L45&amp;$AC$1&amp;fatalities!L46&amp;$AC$1&amp;L$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;L$2</f>
+        <v>7/4/2020,7,4,2020,168,,JU,nn,nnn,73419</v>
+      </c>
+      <c r="AO45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;M45&amp;$AC$1&amp;fatalities!M46&amp;$AC$1&amp;M$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;M$2</f>
+        <v>7/4/2020,7,4,2020,509,9,LU,nn,nnn,409557</v>
+      </c>
+      <c r="AP45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;N45&amp;$AC$1&amp;fatalities!N46&amp;$AC$1&amp;N$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;N$2</f>
+        <v>7/4/2020,7,4,2020,492,,NE,nn,nnn,176850</v>
+      </c>
+      <c r="AQ45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;O45&amp;$AC$1&amp;fatalities!O46&amp;$AC$1&amp;O$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;O$2</f>
+        <v>7/4/2020,7,4,2020,87,0,NW,nn,nnn,43223</v>
+      </c>
+      <c r="AR45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;P45&amp;$AC$1&amp;fatalities!P46&amp;$AC$1&amp;P$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;P$2</f>
+        <v>7/4/2020,7,4,2020,60,0,OW,nn,nnn,37841</v>
+      </c>
+      <c r="AS45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;Q45&amp;$AC$1&amp;fatalities!Q46&amp;$AC$1&amp;Q$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;Q$2</f>
+        <v>7/4/2020,7,4,2020,557,13,SG,nn,nnn,507697</v>
+      </c>
+      <c r="AT45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;R45&amp;$AC$1&amp;fatalities!R46&amp;$AC$1&amp;R$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;R$2</f>
+        <v>7/4/2020,7,4,2020,50,1,SH,nn,nnn,81991</v>
+      </c>
+      <c r="AU45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;S45&amp;$AC$1&amp;fatalities!S46&amp;$AC$1&amp;S$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;S$2</f>
+        <v>7/4/2020,7,4,2020,264,3,SO,nn,nnn,273194</v>
+      </c>
+      <c r="AV45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;T45&amp;$AC$1&amp;fatalities!T46&amp;$AC$1&amp;T$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;T$2</f>
+        <v>7/4/2020,7,4,2020,185,7,SZ,nn,nnn,159165</v>
+      </c>
+      <c r="AW45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;U45&amp;$AC$1&amp;fatalities!U46&amp;$AC$1&amp;U$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;U$2</f>
+        <v>7/4/2020,7,4,2020,221,8,TG,nn,nnn,276472</v>
+      </c>
+      <c r="AX45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;V45&amp;$AC$1&amp;fatalities!V46&amp;$AC$1&amp;V$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;V$2</f>
+        <v>7/4/2020,7,4,2020,2599,198,TI,nn,nnn,353343</v>
+      </c>
+      <c r="AY45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;W45&amp;$AC$1&amp;fatalities!W46&amp;$AC$1&amp;W$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;W$2</f>
+        <v>7/4/2020,7,4,2020,68,2,UR,nn,nnn,36433</v>
+      </c>
+      <c r="AZ45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;X45&amp;$AC$1&amp;fatalities!X46&amp;$AC$1&amp;X$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;X$2</f>
+        <v>7/4/2020,7,4,2020,4235,172,VD,nn,nnn,799145</v>
+      </c>
+      <c r="BA45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;Y45&amp;$AC$1&amp;fatalities!Y46&amp;$AC$1&amp;Y$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;Y$2</f>
+        <v>7/4/2020,7,4,2020,1436,61,VS,nn,nnn,343955</v>
+      </c>
+      <c r="BB45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;Z45&amp;$AC$1&amp;fatalities!Z46&amp;$AC$1&amp;Z$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;Z$2</f>
+        <v>7/4/2020,7,4,2020,157,3,ZG,nn,nnn,126837</v>
+      </c>
+      <c r="BC45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;AA45&amp;$AC$1&amp;fatalities!AA46&amp;$AC$1&amp;AA$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AA$2</f>
+        <v>7/4/2020,7,4,2020,2719,52,ZH,nn,nnn,1520968</v>
+      </c>
+      <c r="BD45" s="3" t="str">
+        <f>$AC45&amp;$AC$1&amp;AB45&amp;$AC$1&amp;fatalities!AB46&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
+        <v>7/4/2020,7,4,2020,22841,856,CH,nn,nnn,8543707</v>
+      </c>
     </row>
     <row r="46" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="56"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="57"/>
+      <c r="A46" s="56">
+        <v>43929</v>
+      </c>
+      <c r="B46" s="57">
+        <v>788</v>
+      </c>
+      <c r="C46" s="57">
+        <v>23</v>
+      </c>
+      <c r="D46" s="57">
+        <v>72</v>
+      </c>
+      <c r="E46" s="57">
+        <v>1286</v>
+      </c>
+      <c r="F46" s="57">
+        <v>694</v>
+      </c>
+      <c r="G46" s="57">
+        <v>834</v>
+      </c>
+      <c r="H46" s="57">
+        <v>756</v>
+      </c>
       <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
+      <c r="J46" s="57">
+        <v>64</v>
+      </c>
       <c r="K46" s="57"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="57"/>
+      <c r="L46" s="57">
+        <v>174</v>
+      </c>
+      <c r="M46" s="57">
+        <v>527</v>
+      </c>
       <c r="N46" s="57"/>
-      <c r="O46" s="57"/>
-      <c r="P46" s="57"/>
-      <c r="Q46" s="57"/>
-      <c r="R46" s="57"/>
-      <c r="S46" s="57"/>
-      <c r="T46" s="57"/>
-      <c r="U46" s="57"/>
-      <c r="V46" s="57"/>
-      <c r="W46" s="57"/>
+      <c r="O46" s="57">
+        <v>93</v>
+      </c>
+      <c r="P46" s="57">
+        <v>61</v>
+      </c>
+      <c r="Q46" s="57">
+        <v>578</v>
+      </c>
+      <c r="R46" s="57">
+        <v>50</v>
+      </c>
+      <c r="S46" s="57">
+        <v>276</v>
+      </c>
+      <c r="T46" s="57">
+        <v>196</v>
+      </c>
+      <c r="U46" s="57">
+        <v>236</v>
+      </c>
+      <c r="V46" s="44">
+        <v>2659</v>
+      </c>
+      <c r="W46" s="57">
+        <v>72</v>
+      </c>
       <c r="X46" s="57"/>
-      <c r="Y46" s="57"/>
-      <c r="Z46" s="57"/>
-      <c r="AA46" s="57"/>
-      <c r="AB46" s="57"/>
+      <c r="Y46" s="57">
+        <v>1484</v>
+      </c>
+      <c r="Z46" s="57">
+        <v>162</v>
+      </c>
+      <c r="AA46" s="57">
+        <v>2807</v>
+      </c>
+      <c r="AB46" s="57">
+        <v>23280</v>
+      </c>
+      <c r="AC46" s="15" t="str">
+        <f t="shared" ref="AC46" si="10">DAY(A46)&amp;"/"&amp;MONTH(A46)&amp;"/"&amp;YEAR(A46)&amp;$AC$1&amp;DAY(A46)&amp;$AC$1&amp;MONTH(A46)&amp;$AC$1&amp;YEAR(A46)</f>
+        <v>8/4/2020,8,4,2020</v>
+      </c>
+      <c r="AD46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;B46&amp;$AC$1&amp;fatalities!B47&amp;$AC$1&amp;B$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;B$2</f>
+        <v>8/4/2020,8,4,2020,788,16,AG,nn,nnn,677387</v>
+      </c>
+      <c r="AE46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;C46&amp;$AC$1&amp;fatalities!C47&amp;$AC$1&amp;C$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;C$2</f>
+        <v>8/4/2020,8,4,2020,23,,AI,nn,nnn,16145</v>
+      </c>
+      <c r="AF46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;D46&amp;$AC$1&amp;fatalities!D47&amp;$AC$1&amp;D$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;D$2</f>
+        <v>8/4/2020,8,4,2020,72,3,AR,nn,nnn,55234</v>
+      </c>
+      <c r="AG46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;E46&amp;$AC$1&amp;fatalities!E47&amp;$AC$1&amp;E$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;E$2</f>
+        <v>8/4/2020,8,4,2020,1286,37,BE,nn,nnn,1034977</v>
+      </c>
+      <c r="AH46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;F46&amp;$AC$1&amp;fatalities!F47&amp;$AC$1&amp;F$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;F$2</f>
+        <v>8/4/2020,8,4,2020,694,21,BL,nn,nnn,288132</v>
+      </c>
+      <c r="AI46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;G46&amp;$AC$1&amp;fatalities!G47&amp;$AC$1&amp;G$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;G$2</f>
+        <v>8/4/2020,8,4,2020,834,31,BS,nn,nnn,194766</v>
+      </c>
+      <c r="AJ46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;H46&amp;$AC$1&amp;fatalities!H47&amp;$AC$1&amp;H$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;H$2</f>
+        <v>8/4/2020,8,4,2020,756,45,FR,nn,nnn,318714</v>
+      </c>
+      <c r="AK46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;I46&amp;$AC$1&amp;fatalities!I47&amp;$AC$1&amp;I$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;I$2</f>
+        <v>8/4/2020,8,4,2020,,,GE,nn,nnn,499480</v>
+      </c>
+      <c r="AL46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;J46&amp;$AC$1&amp;fatalities!J47&amp;$AC$1&amp;J$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;J$2</f>
+        <v>8/4/2020,8,4,2020,64,2,GL,nn,nnn,40403</v>
+      </c>
+      <c r="AM46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;K46&amp;$AC$1&amp;fatalities!K47&amp;$AC$1&amp;K$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;K$2</f>
+        <v>8/4/2020,8,4,2020,,,GR,nn,nnn,198379</v>
+      </c>
+      <c r="AN46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;L46&amp;$AC$1&amp;fatalities!L47&amp;$AC$1&amp;L$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;L$2</f>
+        <v>8/4/2020,8,4,2020,174,,JU,nn,nnn,73419</v>
+      </c>
+      <c r="AO46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;M46&amp;$AC$1&amp;fatalities!M47&amp;$AC$1&amp;M$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;M$2</f>
+        <v>8/4/2020,8,4,2020,527,9,LU,nn,nnn,409557</v>
+      </c>
+      <c r="AP46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;N46&amp;$AC$1&amp;fatalities!N47&amp;$AC$1&amp;N$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;N$2</f>
+        <v>8/4/2020,8,4,2020,,,NE,nn,nnn,176850</v>
+      </c>
+      <c r="AQ46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;O46&amp;$AC$1&amp;fatalities!O47&amp;$AC$1&amp;O$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;O$2</f>
+        <v>8/4/2020,8,4,2020,93,0,NW,nn,nnn,43223</v>
+      </c>
+      <c r="AR46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;P46&amp;$AC$1&amp;fatalities!P47&amp;$AC$1&amp;P$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;P$2</f>
+        <v>8/4/2020,8,4,2020,61,0,OW,nn,nnn,37841</v>
+      </c>
+      <c r="AS46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;Q46&amp;$AC$1&amp;fatalities!Q47&amp;$AC$1&amp;Q$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;Q$2</f>
+        <v>8/4/2020,8,4,2020,578,15,SG,nn,nnn,507697</v>
+      </c>
+      <c r="AT46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;R46&amp;$AC$1&amp;fatalities!R47&amp;$AC$1&amp;R$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;R$2</f>
+        <v>8/4/2020,8,4,2020,50,1,SH,nn,nnn,81991</v>
+      </c>
+      <c r="AU46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;S46&amp;$AC$1&amp;fatalities!S47&amp;$AC$1&amp;S$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;S$2</f>
+        <v>8/4/2020,8,4,2020,276,3,SO,nn,nnn,273194</v>
+      </c>
+      <c r="AV46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;T46&amp;$AC$1&amp;fatalities!T47&amp;$AC$1&amp;T$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;T$2</f>
+        <v>8/4/2020,8,4,2020,196,7,SZ,nn,nnn,159165</v>
+      </c>
+      <c r="AW46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;U46&amp;$AC$1&amp;fatalities!U47&amp;$AC$1&amp;U$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;U$2</f>
+        <v>8/4/2020,8,4,2020,236,8,TG,nn,nnn,276472</v>
+      </c>
+      <c r="AX46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;V46&amp;$AC$1&amp;fatalities!V47&amp;$AC$1&amp;V$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;V$2</f>
+        <v>8/4/2020,8,4,2020,2659,211,TI,nn,nnn,353343</v>
+      </c>
+      <c r="AY46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;W46&amp;$AC$1&amp;fatalities!W47&amp;$AC$1&amp;W$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;W$2</f>
+        <v>8/4/2020,8,4,2020,72,4,UR,nn,nnn,36433</v>
+      </c>
+      <c r="AZ46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;X46&amp;$AC$1&amp;fatalities!X47&amp;$AC$1&amp;X$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;X$2</f>
+        <v>8/4/2020,8,4,2020,,,VD,nn,nnn,799145</v>
+      </c>
+      <c r="BA46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;Y46&amp;$AC$1&amp;fatalities!Y47&amp;$AC$1&amp;Y$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;Y$2</f>
+        <v>8/4/2020,8,4,2020,1484,68,VS,nn,nnn,343955</v>
+      </c>
+      <c r="BB46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;Z46&amp;$AC$1&amp;fatalities!Z47&amp;$AC$1&amp;Z$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;Z$2</f>
+        <v>8/4/2020,8,4,2020,162,3,ZG,nn,nnn,126837</v>
+      </c>
+      <c r="BC46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;AA46&amp;$AC$1&amp;fatalities!AA47&amp;$AC$1&amp;AA$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AA$2</f>
+        <v>8/4/2020,8,4,2020,2807,57,ZH,nn,nnn,1520968</v>
+      </c>
+      <c r="BD46" s="3" t="str">
+        <f>$AC46&amp;$AC$1&amp;AB46&amp;$AC$1&amp;fatalities!AB47&amp;$AC$1&amp;AB$1&amp;$AC$1&amp;"nn"&amp;$AC$1&amp;"nnn"&amp;$AC$1&amp;AB$2</f>
+        <v>8/4/2020,8,4,2020,23280,895,CH,nn,nnn,8543707</v>
+      </c>
     </row>
     <row r="47" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="54"/>
-      <c r="B47" s="55"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="55"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="55"/>
-      <c r="L47" s="55"/>
-      <c r="M47" s="55"/>
-      <c r="N47" s="55"/>
-      <c r="O47" s="55"/>
-      <c r="P47" s="55"/>
-      <c r="Q47" s="55"/>
-      <c r="R47" s="55"/>
-      <c r="S47" s="55"/>
-      <c r="T47" s="55"/>
-      <c r="U47" s="55"/>
-      <c r="V47" s="55"/>
-      <c r="W47" s="55"/>
-      <c r="X47" s="55"/>
-      <c r="Y47" s="55"/>
-      <c r="Z47" s="55"/>
-      <c r="AA47" s="55"/>
-      <c r="AB47" s="55"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="57"/>
+      <c r="M47" s="57"/>
+      <c r="N47" s="57"/>
+      <c r="O47" s="57"/>
+      <c r="P47" s="57"/>
+      <c r="Q47" s="57"/>
+      <c r="R47" s="57"/>
+      <c r="S47" s="57"/>
+      <c r="T47" s="57"/>
+      <c r="U47" s="57"/>
+      <c r="V47" s="57"/>
+      <c r="W47" s="57"/>
+      <c r="X47" s="57"/>
+      <c r="Y47" s="57"/>
+      <c r="Z47" s="57"/>
+      <c r="AA47" s="57"/>
+      <c r="AB47" s="57"/>
+      <c r="AC47" s="57"/>
+      <c r="AD47" s="10"/>
     </row>
     <row r="48" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="56"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="57"/>
-      <c r="H48" s="57"/>
-      <c r="I48" s="57"/>
-      <c r="J48" s="57"/>
-      <c r="K48" s="57"/>
-      <c r="L48" s="57"/>
-      <c r="M48" s="57"/>
-      <c r="N48" s="57"/>
-      <c r="O48" s="57"/>
-      <c r="P48" s="57"/>
-      <c r="Q48" s="57"/>
-      <c r="R48" s="57"/>
-      <c r="S48" s="57"/>
-      <c r="T48" s="57"/>
-      <c r="U48" s="57"/>
-      <c r="V48" s="57"/>
-      <c r="W48" s="57"/>
-      <c r="X48" s="57"/>
-      <c r="Y48" s="57"/>
-      <c r="Z48" s="57"/>
-      <c r="AA48" s="57"/>
-      <c r="AB48" s="57"/>
-    </row>
-    <row r="49" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="54"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="55"/>
-      <c r="K49" s="55"/>
-      <c r="L49" s="55"/>
-      <c r="M49" s="55"/>
-      <c r="N49" s="55"/>
-      <c r="O49" s="55"/>
-      <c r="P49" s="55"/>
-      <c r="Q49" s="55"/>
-      <c r="R49" s="55"/>
-      <c r="S49" s="55"/>
-      <c r="T49" s="55"/>
-      <c r="U49" s="55"/>
-      <c r="V49" s="55"/>
-      <c r="W49" s="55"/>
-      <c r="X49" s="55"/>
-      <c r="Y49" s="55"/>
-      <c r="Z49" s="55"/>
-      <c r="AA49" s="55"/>
-      <c r="AB49" s="55"/>
-    </row>
-    <row r="50" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="56"/>
-      <c r="B50" s="57"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="57"/>
-      <c r="M50" s="57"/>
-      <c r="N50" s="57"/>
-      <c r="O50" s="57"/>
-      <c r="P50" s="57"/>
-      <c r="Q50" s="57"/>
-      <c r="R50" s="57"/>
-      <c r="S50" s="57"/>
-      <c r="T50" s="57"/>
-      <c r="U50" s="57"/>
-      <c r="V50" s="57"/>
-      <c r="W50" s="57"/>
-      <c r="X50" s="57"/>
-      <c r="Y50" s="57"/>
-      <c r="Z50" s="57"/>
-      <c r="AA50" s="57"/>
-      <c r="AB50" s="57"/>
-    </row>
-    <row r="51" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="54"/>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="55"/>
-      <c r="H51" s="55"/>
-      <c r="I51" s="55"/>
-      <c r="J51" s="55"/>
-      <c r="K51" s="55"/>
-      <c r="L51" s="55"/>
-      <c r="M51" s="55"/>
-      <c r="N51" s="55"/>
-      <c r="O51" s="55"/>
-      <c r="P51" s="55"/>
-      <c r="Q51" s="55"/>
-      <c r="R51" s="55"/>
-      <c r="S51" s="55"/>
-      <c r="T51" s="55"/>
-      <c r="U51" s="55"/>
-      <c r="V51" s="55"/>
-      <c r="W51" s="55"/>
-      <c r="X51" s="55"/>
-      <c r="Y51" s="55"/>
-      <c r="Z51" s="55"/>
-      <c r="AA51" s="55"/>
-      <c r="AB51" s="55"/>
-    </row>
-    <row r="52" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="56"/>
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57"/>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="57"/>
-      <c r="N52" s="57"/>
-      <c r="O52" s="57"/>
-      <c r="P52" s="57"/>
-      <c r="Q52" s="57"/>
-      <c r="R52" s="57"/>
-      <c r="S52" s="57"/>
-      <c r="T52" s="57"/>
-      <c r="U52" s="57"/>
-      <c r="V52" s="57"/>
-      <c r="W52" s="57"/>
-      <c r="X52" s="57"/>
-      <c r="Y52" s="57"/>
-      <c r="Z52" s="57"/>
-      <c r="AA52" s="57"/>
-      <c r="AB52" s="57"/>
-    </row>
-    <row r="53" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="54"/>
-      <c r="B53" s="55"/>
-      <c r="C53" s="55"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="55"/>
-      <c r="H53" s="55"/>
-      <c r="I53" s="55"/>
-      <c r="J53" s="55"/>
-      <c r="K53" s="55"/>
-      <c r="L53" s="55"/>
-      <c r="M53" s="55"/>
-      <c r="N53" s="55"/>
-      <c r="O53" s="55"/>
-      <c r="P53" s="55"/>
-      <c r="Q53" s="55"/>
-      <c r="R53" s="55"/>
-      <c r="S53" s="55"/>
-      <c r="T53" s="55"/>
-      <c r="U53" s="55"/>
-      <c r="V53" s="55"/>
-      <c r="W53" s="55"/>
-      <c r="X53" s="55"/>
-      <c r="Y53" s="55"/>
-      <c r="Z53" s="55"/>
-      <c r="AA53" s="55"/>
-      <c r="AB53" s="55"/>
-    </row>
-    <row r="54" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="56"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="57"/>
-      <c r="H54" s="57"/>
-      <c r="I54" s="57"/>
-      <c r="J54" s="57"/>
-      <c r="K54" s="57"/>
-      <c r="L54" s="57"/>
-      <c r="M54" s="57"/>
-      <c r="N54" s="57"/>
-      <c r="O54" s="57"/>
-      <c r="P54" s="57"/>
-      <c r="Q54" s="57"/>
-      <c r="R54" s="57"/>
-      <c r="S54" s="57"/>
-      <c r="T54" s="57"/>
-      <c r="U54" s="57"/>
-      <c r="V54" s="57"/>
-      <c r="W54" s="57"/>
-      <c r="X54" s="57"/>
-      <c r="Y54" s="57"/>
-      <c r="Z54" s="57"/>
-      <c r="AA54" s="57"/>
-      <c r="AB54" s="57"/>
-    </row>
-    <row r="55" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="54"/>
-      <c r="B55" s="55"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="55"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
-      <c r="G55" s="55"/>
-      <c r="H55" s="55"/>
-      <c r="I55" s="55"/>
-      <c r="J55" s="55"/>
-      <c r="K55" s="55"/>
-      <c r="L55" s="55"/>
-      <c r="M55" s="55"/>
-      <c r="N55" s="55"/>
-      <c r="O55" s="55"/>
-      <c r="P55" s="55"/>
-      <c r="Q55" s="55"/>
-      <c r="R55" s="55"/>
-      <c r="S55" s="55"/>
-      <c r="T55" s="55"/>
-      <c r="U55" s="55"/>
-      <c r="V55" s="55"/>
-      <c r="W55" s="55"/>
-      <c r="X55" s="55"/>
-      <c r="Y55" s="55"/>
-      <c r="Z55" s="55"/>
-      <c r="AA55" s="55"/>
-      <c r="AB55" s="55"/>
-    </row>
-    <row r="56" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="56"/>
-      <c r="B56" s="57"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="57"/>
-      <c r="E56" s="57"/>
-      <c r="F56" s="57"/>
-      <c r="G56" s="57"/>
-      <c r="H56" s="57"/>
-      <c r="I56" s="57"/>
-      <c r="J56" s="57"/>
-      <c r="K56" s="57"/>
-      <c r="L56" s="57"/>
-      <c r="M56" s="57"/>
-      <c r="N56" s="57"/>
-      <c r="O56" s="57"/>
-      <c r="P56" s="57"/>
-      <c r="Q56" s="57"/>
-      <c r="R56" s="57"/>
-      <c r="S56" s="57"/>
-      <c r="T56" s="57"/>
-      <c r="U56" s="57"/>
-      <c r="V56" s="57"/>
-      <c r="W56" s="57"/>
-      <c r="X56" s="57"/>
-      <c r="Y56" s="57"/>
-      <c r="Z56" s="57"/>
-      <c r="AA56" s="57"/>
-      <c r="AB56" s="57"/>
-    </row>
-    <row r="57" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="54"/>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="55"/>
-      <c r="H57" s="55"/>
-      <c r="I57" s="55"/>
-      <c r="J57" s="55"/>
-      <c r="K57" s="55"/>
-      <c r="L57" s="55"/>
-      <c r="M57" s="55"/>
-      <c r="N57" s="55"/>
-      <c r="O57" s="55"/>
-      <c r="P57" s="55"/>
-      <c r="Q57" s="55"/>
-      <c r="R57" s="55"/>
-      <c r="S57" s="55"/>
-      <c r="T57" s="55"/>
-      <c r="U57" s="55"/>
-      <c r="V57" s="55"/>
-      <c r="W57" s="55"/>
-      <c r="X57" s="55"/>
-      <c r="Y57" s="55"/>
-      <c r="Z57" s="55"/>
-      <c r="AA57" s="55"/>
-      <c r="AB57" s="55"/>
-    </row>
-    <row r="58" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="56"/>
-      <c r="B58" s="57"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="57"/>
-      <c r="E58" s="57"/>
-      <c r="F58" s="57"/>
-      <c r="G58" s="57"/>
-      <c r="H58" s="57"/>
-      <c r="I58" s="57"/>
-      <c r="J58" s="57"/>
-      <c r="K58" s="57"/>
-      <c r="L58" s="57"/>
-      <c r="M58" s="57"/>
-      <c r="N58" s="57"/>
-      <c r="O58" s="57"/>
-      <c r="P58" s="57"/>
-      <c r="Q58" s="57"/>
-      <c r="R58" s="57"/>
-      <c r="S58" s="57"/>
-      <c r="T58" s="57"/>
-      <c r="U58" s="57"/>
-      <c r="V58" s="57"/>
-      <c r="W58" s="57"/>
-      <c r="X58" s="57"/>
-      <c r="Y58" s="57"/>
-      <c r="Z58" s="57"/>
-      <c r="AA58" s="57"/>
-      <c r="AB58" s="57"/>
-    </row>
-    <row r="59" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="54"/>
-      <c r="B59" s="55"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="55"/>
-      <c r="H59" s="55"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
-      <c r="K59" s="55"/>
-      <c r="L59" s="55"/>
-      <c r="M59" s="55"/>
-      <c r="N59" s="55"/>
-      <c r="O59" s="55"/>
-      <c r="P59" s="55"/>
-      <c r="Q59" s="55"/>
-      <c r="R59" s="55"/>
-      <c r="S59" s="55"/>
-      <c r="T59" s="55"/>
-      <c r="U59" s="55"/>
-      <c r="V59" s="55"/>
-      <c r="W59" s="55"/>
-      <c r="X59" s="55"/>
-      <c r="Y59" s="55"/>
-      <c r="Z59" s="55"/>
-      <c r="AA59" s="55"/>
-      <c r="AB59" s="55"/>
-    </row>
-    <row r="60" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="56"/>
-      <c r="B60" s="57"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="57"/>
-      <c r="H60" s="57"/>
-      <c r="I60" s="57"/>
-      <c r="J60" s="57"/>
-      <c r="K60" s="57"/>
-      <c r="L60" s="57"/>
-      <c r="M60" s="57"/>
-      <c r="N60" s="57"/>
-      <c r="O60" s="57"/>
-      <c r="P60" s="57"/>
-      <c r="Q60" s="57"/>
-      <c r="R60" s="57"/>
-      <c r="S60" s="57"/>
-      <c r="T60" s="57"/>
-      <c r="U60" s="57"/>
-      <c r="V60" s="57"/>
-      <c r="W60" s="57"/>
-      <c r="X60" s="57"/>
-      <c r="Y60" s="57"/>
-      <c r="Z60" s="57"/>
-      <c r="AA60" s="57"/>
-      <c r="AB60" s="57"/>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="U61" s="45"/>
-      <c r="V61"/>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="U62" s="45"/>
-      <c r="V62"/>
+      <c r="A48" s="58"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="55"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="55"/>
+      <c r="L48" s="55"/>
+      <c r="M48" s="55"/>
+      <c r="N48" s="55"/>
+      <c r="O48" s="55"/>
+      <c r="P48" s="55"/>
+      <c r="Q48" s="55"/>
+      <c r="R48" s="55"/>
+      <c r="S48" s="55"/>
+      <c r="T48" s="55"/>
+      <c r="U48" s="55"/>
+      <c r="V48" s="55"/>
+      <c r="W48" s="55"/>
+      <c r="X48" s="55"/>
+      <c r="Y48" s="55"/>
+      <c r="Z48" s="55"/>
+      <c r="AA48" s="55"/>
+      <c r="AB48" s="55"/>
+      <c r="AC48" s="55"/>
+    </row>
+    <row r="49" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="58"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="57"/>
+      <c r="K49" s="57"/>
+      <c r="L49" s="57"/>
+      <c r="M49" s="57"/>
+      <c r="N49" s="57"/>
+      <c r="O49" s="57"/>
+      <c r="P49" s="57"/>
+      <c r="Q49" s="57"/>
+      <c r="R49" s="57"/>
+      <c r="S49" s="57"/>
+      <c r="T49" s="57"/>
+      <c r="U49" s="57"/>
+      <c r="V49" s="57"/>
+      <c r="W49" s="57"/>
+      <c r="X49" s="57"/>
+      <c r="Y49" s="57"/>
+      <c r="Z49" s="57"/>
+      <c r="AA49" s="57"/>
+      <c r="AB49" s="57"/>
+      <c r="AC49" s="57"/>
+    </row>
+    <row r="50" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="58"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="55"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="55"/>
+      <c r="K50" s="55"/>
+      <c r="L50" s="55"/>
+      <c r="M50" s="55"/>
+      <c r="N50" s="55"/>
+      <c r="O50" s="55"/>
+      <c r="P50" s="55"/>
+      <c r="Q50" s="55"/>
+      <c r="R50" s="55"/>
+      <c r="S50" s="55"/>
+      <c r="T50" s="55"/>
+      <c r="U50" s="55"/>
+      <c r="V50" s="55"/>
+      <c r="W50" s="55"/>
+      <c r="X50" s="55"/>
+      <c r="Y50" s="55"/>
+      <c r="Z50" s="55"/>
+      <c r="AA50" s="55"/>
+      <c r="AB50" s="55"/>
+      <c r="AC50" s="55"/>
+    </row>
+    <row r="51" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="58"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
+      <c r="L51" s="57"/>
+      <c r="M51" s="57"/>
+      <c r="N51" s="57"/>
+      <c r="O51" s="57"/>
+      <c r="P51" s="57"/>
+      <c r="Q51" s="57"/>
+      <c r="R51" s="57"/>
+      <c r="S51" s="57"/>
+      <c r="T51" s="57"/>
+      <c r="U51" s="57"/>
+      <c r="V51" s="57"/>
+      <c r="W51" s="57"/>
+      <c r="X51" s="57"/>
+      <c r="Y51" s="57"/>
+      <c r="Z51" s="57"/>
+      <c r="AA51" s="57"/>
+      <c r="AB51" s="57"/>
+      <c r="AC51" s="57"/>
+    </row>
+    <row r="52" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="58"/>
+      <c r="B52" s="54"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="55"/>
+      <c r="H52" s="55"/>
+      <c r="I52" s="55"/>
+      <c r="J52" s="55"/>
+      <c r="K52" s="55"/>
+      <c r="L52" s="55"/>
+      <c r="M52" s="55"/>
+      <c r="N52" s="55"/>
+      <c r="O52" s="55"/>
+      <c r="P52" s="55"/>
+      <c r="Q52" s="55"/>
+      <c r="R52" s="55"/>
+      <c r="S52" s="55"/>
+      <c r="T52" s="55"/>
+      <c r="U52" s="55"/>
+      <c r="V52" s="55"/>
+      <c r="W52" s="55"/>
+      <c r="X52" s="55"/>
+      <c r="Y52" s="55"/>
+      <c r="Z52" s="55"/>
+      <c r="AA52" s="55"/>
+      <c r="AB52" s="55"/>
+      <c r="AC52" s="55"/>
+    </row>
+    <row r="53" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="58"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="57"/>
+      <c r="J53" s="57"/>
+      <c r="K53" s="57"/>
+      <c r="L53" s="57"/>
+      <c r="M53" s="57"/>
+      <c r="N53" s="57"/>
+      <c r="O53" s="57"/>
+      <c r="P53" s="57"/>
+      <c r="Q53" s="57"/>
+      <c r="R53" s="57"/>
+      <c r="S53" s="57"/>
+      <c r="T53" s="57"/>
+      <c r="U53" s="57"/>
+      <c r="V53" s="57"/>
+      <c r="W53" s="57"/>
+      <c r="X53" s="57"/>
+      <c r="Y53" s="57"/>
+      <c r="Z53" s="57"/>
+      <c r="AA53" s="57"/>
+      <c r="AB53" s="57"/>
+      <c r="AC53" s="57"/>
+    </row>
+    <row r="54" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="58"/>
+      <c r="B54" s="54"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="55"/>
+      <c r="G54" s="55"/>
+      <c r="H54" s="55"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="55"/>
+      <c r="L54" s="55"/>
+      <c r="M54" s="55"/>
+      <c r="N54" s="55"/>
+      <c r="O54" s="55"/>
+      <c r="P54" s="55"/>
+      <c r="Q54" s="55"/>
+      <c r="R54" s="55"/>
+      <c r="S54" s="55"/>
+      <c r="T54" s="55"/>
+      <c r="U54" s="55"/>
+      <c r="V54" s="55"/>
+      <c r="W54" s="55"/>
+      <c r="X54" s="55"/>
+      <c r="Y54" s="55"/>
+      <c r="Z54" s="55"/>
+      <c r="AA54" s="55"/>
+      <c r="AB54" s="55"/>
+      <c r="AC54" s="55"/>
+    </row>
+    <row r="55" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="58"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="57"/>
+      <c r="G55" s="57"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="57"/>
+      <c r="J55" s="57"/>
+      <c r="K55" s="57"/>
+      <c r="L55" s="57"/>
+      <c r="M55" s="57"/>
+      <c r="N55" s="57"/>
+      <c r="O55" s="57"/>
+      <c r="P55" s="57"/>
+      <c r="Q55" s="57"/>
+      <c r="R55" s="57"/>
+      <c r="S55" s="57"/>
+      <c r="T55" s="57"/>
+      <c r="U55" s="57"/>
+      <c r="V55" s="57"/>
+      <c r="W55" s="57"/>
+      <c r="X55" s="57"/>
+      <c r="Y55" s="57"/>
+      <c r="Z55" s="57"/>
+      <c r="AA55" s="57"/>
+      <c r="AB55" s="57"/>
+      <c r="AC55" s="57"/>
+    </row>
+    <row r="56" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="58"/>
+      <c r="B56" s="54"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="55"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="55"/>
+      <c r="I56" s="55"/>
+      <c r="J56" s="55"/>
+      <c r="K56" s="55"/>
+      <c r="L56" s="55"/>
+      <c r="M56" s="55"/>
+      <c r="N56" s="55"/>
+      <c r="O56" s="55"/>
+      <c r="P56" s="55"/>
+      <c r="Q56" s="55"/>
+      <c r="R56" s="55"/>
+      <c r="S56" s="55"/>
+      <c r="T56" s="55"/>
+      <c r="U56" s="55"/>
+      <c r="V56" s="55"/>
+      <c r="W56" s="55"/>
+      <c r="X56" s="55"/>
+      <c r="Y56" s="55"/>
+      <c r="Z56" s="55"/>
+      <c r="AA56" s="55"/>
+      <c r="AB56" s="55"/>
+      <c r="AC56" s="55"/>
+    </row>
+    <row r="57" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="58"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="57"/>
+      <c r="F57" s="57"/>
+      <c r="G57" s="57"/>
+      <c r="H57" s="57"/>
+      <c r="I57" s="57"/>
+      <c r="J57" s="57"/>
+      <c r="K57" s="57"/>
+      <c r="L57" s="57"/>
+      <c r="M57" s="57"/>
+      <c r="N57" s="57"/>
+      <c r="O57" s="57"/>
+      <c r="P57" s="57"/>
+      <c r="Q57" s="57"/>
+      <c r="R57" s="57"/>
+      <c r="S57" s="57"/>
+      <c r="T57" s="57"/>
+      <c r="U57" s="57"/>
+      <c r="V57" s="57"/>
+      <c r="W57" s="57"/>
+      <c r="X57" s="57"/>
+      <c r="Y57" s="57"/>
+      <c r="Z57" s="57"/>
+      <c r="AA57" s="57"/>
+      <c r="AB57" s="57"/>
+      <c r="AC57" s="57"/>
+    </row>
+    <row r="58" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="58"/>
+      <c r="B58" s="54"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="55"/>
+      <c r="G58" s="55"/>
+      <c r="H58" s="55"/>
+      <c r="I58" s="55"/>
+      <c r="J58" s="55"/>
+      <c r="K58" s="55"/>
+      <c r="L58" s="55"/>
+      <c r="M58" s="55"/>
+      <c r="N58" s="55"/>
+      <c r="O58" s="55"/>
+      <c r="P58" s="55"/>
+      <c r="Q58" s="55"/>
+      <c r="R58" s="55"/>
+      <c r="S58" s="55"/>
+      <c r="T58" s="55"/>
+      <c r="U58" s="55"/>
+      <c r="V58" s="55"/>
+      <c r="W58" s="55"/>
+      <c r="X58" s="55"/>
+      <c r="Y58" s="55"/>
+      <c r="Z58" s="55"/>
+      <c r="AA58" s="55"/>
+      <c r="AB58" s="55"/>
+      <c r="AC58" s="55"/>
+    </row>
+    <row r="59" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="58"/>
+      <c r="B59" s="56"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="57"/>
+      <c r="F59" s="57"/>
+      <c r="G59" s="57"/>
+      <c r="H59" s="57"/>
+      <c r="I59" s="57"/>
+      <c r="J59" s="57"/>
+      <c r="K59" s="57"/>
+      <c r="L59" s="57"/>
+      <c r="M59" s="57"/>
+      <c r="N59" s="57"/>
+      <c r="O59" s="57"/>
+      <c r="P59" s="57"/>
+      <c r="Q59" s="57"/>
+      <c r="R59" s="57"/>
+      <c r="S59" s="57"/>
+      <c r="T59" s="57"/>
+      <c r="U59" s="57"/>
+      <c r="V59" s="57"/>
+      <c r="W59" s="57"/>
+      <c r="X59" s="57"/>
+      <c r="Y59" s="57"/>
+      <c r="Z59" s="57"/>
+      <c r="AA59" s="57"/>
+      <c r="AB59" s="57"/>
+      <c r="AC59" s="57"/>
+    </row>
+    <row r="60" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="58"/>
+      <c r="B60" s="54"/>
+      <c r="C60" s="55"/>
+      <c r="D60" s="55"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="55"/>
+      <c r="G60" s="55"/>
+      <c r="H60" s="55"/>
+      <c r="I60" s="55"/>
+      <c r="J60" s="55"/>
+      <c r="K60" s="55"/>
+      <c r="L60" s="55"/>
+      <c r="M60" s="55"/>
+      <c r="N60" s="55"/>
+      <c r="O60" s="55"/>
+      <c r="P60" s="55"/>
+      <c r="Q60" s="55"/>
+      <c r="R60" s="55"/>
+      <c r="S60" s="55"/>
+      <c r="T60" s="55"/>
+      <c r="U60" s="55"/>
+      <c r="V60" s="55"/>
+      <c r="W60" s="55"/>
+      <c r="X60" s="55"/>
+      <c r="Y60" s="55"/>
+      <c r="Z60" s="55"/>
+      <c r="AA60" s="55"/>
+      <c r="AB60" s="55"/>
+      <c r="AC60" s="55"/>
+    </row>
+    <row r="61" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="58"/>
+      <c r="B61" s="56"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="57"/>
+      <c r="G61" s="57"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="57"/>
+      <c r="J61" s="57"/>
+      <c r="K61" s="57"/>
+      <c r="L61" s="57"/>
+      <c r="M61" s="57"/>
+      <c r="N61" s="57"/>
+      <c r="O61" s="57"/>
+      <c r="P61" s="57"/>
+      <c r="Q61" s="57"/>
+      <c r="R61" s="57"/>
+      <c r="S61" s="57"/>
+      <c r="T61" s="57"/>
+      <c r="U61" s="57"/>
+      <c r="V61" s="57"/>
+      <c r="W61" s="57"/>
+      <c r="X61" s="57"/>
+      <c r="Y61" s="57"/>
+      <c r="Z61" s="57"/>
+      <c r="AA61" s="57"/>
+      <c r="AB61" s="57"/>
+      <c r="AC61" s="57"/>
+    </row>
+    <row r="62" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="58"/>
+      <c r="B62" s="54"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="55"/>
+      <c r="J62" s="55"/>
+      <c r="K62" s="55"/>
+      <c r="L62" s="55"/>
+      <c r="M62" s="55"/>
+      <c r="N62" s="55"/>
+      <c r="O62" s="55"/>
+      <c r="P62" s="55"/>
+      <c r="Q62" s="55"/>
+      <c r="R62" s="55"/>
+      <c r="S62" s="55"/>
+      <c r="T62" s="55"/>
+      <c r="U62" s="55"/>
+      <c r="V62" s="55"/>
+      <c r="W62" s="55"/>
+      <c r="X62" s="55"/>
+      <c r="Y62" s="55"/>
+      <c r="Z62" s="55"/>
+      <c r="AA62" s="55"/>
+      <c r="AB62" s="55"/>
+      <c r="AC62" s="55"/>
+    </row>
+    <row r="63" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="58"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="57"/>
+      <c r="F63" s="57"/>
+      <c r="G63" s="57"/>
+      <c r="H63" s="57"/>
+      <c r="I63" s="57"/>
+      <c r="J63" s="57"/>
+      <c r="K63" s="57"/>
+      <c r="L63" s="57"/>
+      <c r="M63" s="57"/>
+      <c r="N63" s="57"/>
+      <c r="O63" s="57"/>
+      <c r="P63" s="57"/>
+      <c r="Q63" s="57"/>
+      <c r="R63" s="57"/>
+      <c r="S63" s="57"/>
+      <c r="T63" s="57"/>
+      <c r="U63" s="57"/>
+      <c r="V63" s="57"/>
+      <c r="W63" s="57"/>
+      <c r="X63" s="57"/>
+      <c r="Y63" s="57"/>
+      <c r="Z63" s="57"/>
+      <c r="AA63" s="57"/>
+      <c r="AB63" s="57"/>
+      <c r="AC63" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13132,11 +13731,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC61"/>
+  <dimension ref="A1:AE66"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V45" sqref="V45"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V47" sqref="V47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13324,11 +13923,11 @@
     <row r="3" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="51">
-        <f>B42/B2</f>
+        <f t="shared" ref="B3:AB3" si="0">B42/B2</f>
         <v>1.7715131822724674E-5</v>
       </c>
       <c r="C3" s="51">
-        <f t="shared" ref="C3:AB3" si="0">C42/C2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D3" s="51">
@@ -13353,7 +13952,7 @@
       </c>
       <c r="I3" s="52">
         <f t="shared" si="0"/>
-        <v>1.5616240890526148E-4</v>
+        <v>1.6016657323616562E-4</v>
       </c>
       <c r="J3" s="51">
         <f t="shared" si="0"/>
@@ -13429,7 +14028,7 @@
       </c>
       <c r="AB3" s="51">
         <f t="shared" si="0"/>
-        <v>7.3621438562909518E-5</v>
+        <v>7.3855528987592855E-5</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -13882,7 +14481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <v>43899</v>
       </c>
@@ -13922,7 +14521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>43900</v>
       </c>
@@ -13964,7 +14563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22">
         <v>43901</v>
       </c>
@@ -14004,7 +14603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>43902</v>
       </c>
@@ -14046,7 +14645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22">
         <v>43903</v>
       </c>
@@ -14088,7 +14687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>43904</v>
       </c>
@@ -14134,7 +14733,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22">
         <v>43905</v>
       </c>
@@ -14178,7 +14777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>43906</v>
       </c>
@@ -14228,7 +14827,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22">
         <v>43907</v>
       </c>
@@ -14274,7 +14873,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>43908</v>
       </c>
@@ -14326,7 +14925,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22">
         <v>43909</v>
       </c>
@@ -14380,7 +14979,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>43910</v>
       </c>
@@ -14438,65 +15037,65 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22">
+    <row r="29" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="56">
         <v>43911</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23">
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57">
         <v>1</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="57">
         <v>3</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="57">
         <v>3</v>
       </c>
-      <c r="G29" s="23">
+      <c r="G29" s="57">
         <v>5</v>
       </c>
-      <c r="H29" s="23">
+      <c r="H29" s="57">
         <v>2</v>
       </c>
-      <c r="I29" s="23">
+      <c r="I29" s="57">
         <v>9</v>
       </c>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23">
+      <c r="J29" s="57"/>
+      <c r="K29" s="57">
         <v>3</v>
       </c>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23">
+      <c r="L29" s="57"/>
+      <c r="M29" s="57">
         <v>1</v>
       </c>
-      <c r="N29" s="23">
+      <c r="N29" s="57">
         <v>4</v>
       </c>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
+      <c r="O29" s="57"/>
+      <c r="P29" s="57"/>
+      <c r="Q29" s="57"/>
+      <c r="R29" s="57"/>
+      <c r="S29" s="57"/>
+      <c r="T29" s="57"/>
+      <c r="U29" s="57"/>
       <c r="V29" s="47">
         <v>28</v>
       </c>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23">
+      <c r="W29" s="57"/>
+      <c r="X29" s="57">
         <v>15</v>
       </c>
-      <c r="Y29" s="23">
+      <c r="Y29" s="57">
         <v>7</v>
       </c>
-      <c r="Z29" s="23"/>
-      <c r="AA29" s="23"/>
-      <c r="AB29" s="23">
+      <c r="Z29" s="57"/>
+      <c r="AA29" s="57"/>
+      <c r="AB29" s="57">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="54">
         <v>43912</v>
       </c>
@@ -14552,7 +15151,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="56">
         <v>43913</v>
       </c>
@@ -14576,7 +15175,7 @@
         <v>4</v>
       </c>
       <c r="I31" s="57">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J31" s="57"/>
       <c r="K31" s="57"/>
@@ -14613,10 +15212,10 @@
         <v>5</v>
       </c>
       <c r="AB31" s="57">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="54">
         <v>43914</v>
       </c>
@@ -14640,7 +15239,7 @@
         <v>5</v>
       </c>
       <c r="I32" s="55">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J32" s="55"/>
       <c r="K32" s="55">
@@ -14679,10 +15278,14 @@
         <v>5</v>
       </c>
       <c r="AB32" s="55">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="AC32" s="10">
+        <f>AB32-AB25</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="56">
         <v>43915</v>
       </c>
@@ -14706,7 +15309,7 @@
         <v>6</v>
       </c>
       <c r="I33" s="57">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J33" s="57"/>
       <c r="K33" s="57">
@@ -14747,10 +15350,10 @@
         <v>7</v>
       </c>
       <c r="AB33" s="57">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="54">
         <v>43916</v>
       </c>
@@ -14774,7 +15377,7 @@
         <v>11</v>
       </c>
       <c r="I34" s="55">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J34" s="55"/>
       <c r="K34" s="55">
@@ -14817,10 +15420,10 @@
         <v>9</v>
       </c>
       <c r="AB34" s="55">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="35" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="56">
         <v>43917</v>
       </c>
@@ -14844,7 +15447,7 @@
         <v>15</v>
       </c>
       <c r="I35" s="57">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="J35" s="57"/>
       <c r="K35" s="57">
@@ -14887,10 +15490,10 @@
         <v>11</v>
       </c>
       <c r="AB35" s="57">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="54">
         <v>43918</v>
       </c>
@@ -14912,7 +15515,7 @@
         <v>15</v>
       </c>
       <c r="I36" s="55">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="J36" s="55">
         <v>1</v>
@@ -14955,10 +15558,10 @@
         <v>15</v>
       </c>
       <c r="AB36" s="55">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="37" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="56">
         <v>43919</v>
       </c>
@@ -14980,7 +15583,7 @@
         <v>16</v>
       </c>
       <c r="I37" s="57">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="J37" s="57"/>
       <c r="K37" s="57"/>
@@ -15021,10 +15624,10 @@
         <v>15</v>
       </c>
       <c r="AB37" s="57">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="38" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="54">
         <v>43920</v>
       </c>
@@ -15048,7 +15651,7 @@
         <v>17</v>
       </c>
       <c r="I38" s="55">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J38" s="55">
         <v>1</v>
@@ -15093,10 +15696,10 @@
         <v>21</v>
       </c>
       <c r="AB38" s="55">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="39" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="56">
         <v>43921</v>
       </c>
@@ -15120,7 +15723,7 @@
         <v>20</v>
       </c>
       <c r="I39" s="57">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="J39" s="57">
         <v>2</v>
@@ -15167,10 +15770,14 @@
         <v>25</v>
       </c>
       <c r="AB39" s="57">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="40" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+      <c r="AC39" s="10">
+        <f>AB39-AB32</f>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="54">
         <v>43922</v>
       </c>
@@ -15194,7 +15801,7 @@
         <v>23</v>
       </c>
       <c r="I40" s="55">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J40" s="55">
         <v>2</v>
@@ -15245,10 +15852,10 @@
         <v>29</v>
       </c>
       <c r="AB40" s="55">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="41" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="56">
         <v>43923</v>
       </c>
@@ -15272,7 +15879,7 @@
         <v>26</v>
       </c>
       <c r="I41" s="57">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J41" s="57">
         <v>2</v>
@@ -15323,10 +15930,10 @@
         <v>36</v>
       </c>
       <c r="AB41" s="57">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="42" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="54">
         <v>43924</v>
       </c>
@@ -15350,7 +15957,7 @@
         <v>31</v>
       </c>
       <c r="I42" s="55">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J42" s="55">
         <v>2</v>
@@ -15401,11 +16008,11 @@
         <v>38</v>
       </c>
       <c r="AB42" s="55">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="AC42"/>
     </row>
-    <row r="43" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="56">
         <v>43925</v>
       </c>
@@ -15427,7 +16034,7 @@
         <v>37</v>
       </c>
       <c r="I43" s="57">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="J43" s="57"/>
       <c r="K43" s="57"/>
@@ -15476,10 +16083,10 @@
         <v>41</v>
       </c>
       <c r="AB43" s="57">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="44" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="54">
         <v>43926</v>
       </c>
@@ -15501,7 +16108,7 @@
         <v>40</v>
       </c>
       <c r="I44" s="55">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J44" s="55"/>
       <c r="K44" s="55">
@@ -15550,11 +16157,11 @@
         <v>45</v>
       </c>
       <c r="AB44" s="55">
-        <v>738</v>
+        <v>746</v>
       </c>
       <c r="AC44" s="10"/>
     </row>
-    <row r="45" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="56">
         <v>43927</v>
       </c>
@@ -15574,18 +16181,24 @@
       <c r="G45" s="57">
         <v>26</v>
       </c>
-      <c r="H45" s="57"/>
-      <c r="I45" s="57"/>
+      <c r="H45" s="57">
+        <v>41</v>
+      </c>
+      <c r="I45" s="57">
+        <v>111</v>
+      </c>
       <c r="J45" s="57">
         <v>2</v>
       </c>
-      <c r="K45" s="57"/>
+      <c r="K45" s="57">
+        <v>31</v>
+      </c>
       <c r="L45" s="57"/>
       <c r="M45" s="57">
         <v>9</v>
       </c>
       <c r="N45" s="57">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="O45" s="57">
         <v>0</v>
@@ -15596,7 +16209,9 @@
       <c r="Q45" s="57">
         <v>11</v>
       </c>
-      <c r="R45" s="57"/>
+      <c r="R45" s="57">
+        <v>1</v>
+      </c>
       <c r="S45" s="57">
         <v>3</v>
       </c>
@@ -15612,7 +16227,9 @@
       <c r="W45" s="57">
         <v>2</v>
       </c>
-      <c r="X45" s="57"/>
+      <c r="X45" s="57">
+        <v>160</v>
+      </c>
       <c r="Y45" s="57">
         <v>56</v>
       </c>
@@ -15623,73 +16240,173 @@
         <v>48</v>
       </c>
       <c r="AB45" s="57">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="46" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
-      <c r="B46" s="55"/>
+        <v>802</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="54">
+        <v>43928</v>
+      </c>
+      <c r="B46" s="55">
+        <v>16</v>
+      </c>
       <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
+      <c r="D46" s="55">
+        <v>3</v>
+      </c>
+      <c r="E46" s="55">
+        <v>33</v>
+      </c>
+      <c r="F46" s="55">
+        <v>19</v>
+      </c>
+      <c r="G46" s="55">
+        <v>28</v>
+      </c>
+      <c r="H46" s="55">
+        <v>44</v>
+      </c>
+      <c r="I46" s="55">
+        <v>118</v>
+      </c>
+      <c r="J46" s="55">
+        <v>2</v>
+      </c>
+      <c r="K46" s="55">
+        <v>34</v>
+      </c>
       <c r="L46" s="55"/>
-      <c r="M46" s="55"/>
+      <c r="M46" s="55">
+        <v>9</v>
+      </c>
       <c r="N46" s="55"/>
-      <c r="O46" s="55"/>
-      <c r="P46" s="55"/>
-      <c r="Q46" s="55"/>
-      <c r="R46" s="55"/>
-      <c r="S46" s="55"/>
-      <c r="T46" s="55"/>
-      <c r="U46" s="55"/>
-      <c r="V46" s="55"/>
-      <c r="W46" s="55"/>
-      <c r="X46" s="55"/>
-      <c r="Y46" s="55"/>
-      <c r="Z46" s="55"/>
-      <c r="AA46" s="55"/>
-      <c r="AB46" s="55"/>
-      <c r="AC46" s="10"/>
-    </row>
-    <row r="47" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="56"/>
-      <c r="B47" s="57"/>
+      <c r="O46" s="55">
+        <v>0</v>
+      </c>
+      <c r="P46" s="55">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="55">
+        <v>13</v>
+      </c>
+      <c r="R46" s="55">
+        <v>1</v>
+      </c>
+      <c r="S46" s="55">
+        <v>3</v>
+      </c>
+      <c r="T46" s="55">
+        <v>7</v>
+      </c>
+      <c r="U46" s="55">
+        <v>8</v>
+      </c>
+      <c r="V46" s="47">
+        <v>198</v>
+      </c>
+      <c r="W46" s="55">
+        <v>2</v>
+      </c>
+      <c r="X46" s="55">
+        <v>172</v>
+      </c>
+      <c r="Y46" s="55">
+        <v>61</v>
+      </c>
+      <c r="Z46" s="55">
+        <v>3</v>
+      </c>
+      <c r="AA46" s="55">
+        <v>52</v>
+      </c>
+      <c r="AB46" s="55">
+        <v>856</v>
+      </c>
+      <c r="AC46" s="10">
+        <f>AB46-AB39</f>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="56">
+        <v>43929</v>
+      </c>
+      <c r="B47" s="57">
+        <v>16</v>
+      </c>
       <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57"/>
+      <c r="D47" s="57">
+        <v>3</v>
+      </c>
+      <c r="E47" s="57">
+        <v>37</v>
+      </c>
+      <c r="F47" s="57">
+        <v>21</v>
+      </c>
+      <c r="G47" s="57">
+        <v>31</v>
+      </c>
+      <c r="H47" s="57">
+        <v>45</v>
+      </c>
       <c r="I47" s="57"/>
-      <c r="J47" s="57"/>
+      <c r="J47" s="57">
+        <v>2</v>
+      </c>
       <c r="K47" s="57"/>
       <c r="L47" s="57"/>
-      <c r="M47" s="57"/>
+      <c r="M47" s="57">
+        <v>9</v>
+      </c>
       <c r="N47" s="57"/>
-      <c r="O47" s="57"/>
-      <c r="P47" s="57"/>
-      <c r="Q47" s="57"/>
-      <c r="R47" s="57"/>
-      <c r="S47" s="57"/>
-      <c r="T47" s="57"/>
-      <c r="U47" s="57"/>
-      <c r="V47" s="57"/>
-      <c r="W47" s="57"/>
+      <c r="O47" s="57">
+        <v>0</v>
+      </c>
+      <c r="P47" s="57">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="57">
+        <v>15</v>
+      </c>
+      <c r="R47" s="57">
+        <v>1</v>
+      </c>
+      <c r="S47" s="57">
+        <v>3</v>
+      </c>
+      <c r="T47" s="57">
+        <v>7</v>
+      </c>
+      <c r="U47" s="57">
+        <v>8</v>
+      </c>
+      <c r="V47" s="47">
+        <v>211</v>
+      </c>
+      <c r="W47" s="57">
+        <v>4</v>
+      </c>
       <c r="X47" s="57"/>
-      <c r="Y47" s="57"/>
-      <c r="Z47" s="57"/>
-      <c r="AA47" s="57"/>
-      <c r="AB47" s="57"/>
-    </row>
-    <row r="48" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
-      <c r="B48" s="55"/>
+      <c r="Y47" s="57">
+        <v>68</v>
+      </c>
+      <c r="Z47" s="57">
+        <v>3</v>
+      </c>
+      <c r="AA47" s="57">
+        <v>57</v>
+      </c>
+      <c r="AB47" s="57">
+        <v>895</v>
+      </c>
+      <c r="AC47" s="57"/>
+      <c r="AD47" s="10"/>
+      <c r="AE47" s="10"/>
+    </row>
+    <row r="48" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="58"/>
+      <c r="B48" s="54"/>
       <c r="C48" s="55"/>
       <c r="D48" s="55"/>
       <c r="E48" s="55"/>
@@ -15716,10 +16433,11 @@
       <c r="Z48" s="55"/>
       <c r="AA48" s="55"/>
       <c r="AB48" s="55"/>
-    </row>
-    <row r="49" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="56"/>
-      <c r="B49" s="57"/>
+      <c r="AC48" s="55"/>
+    </row>
+    <row r="49" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="58"/>
+      <c r="B49" s="56"/>
       <c r="C49" s="57"/>
       <c r="D49" s="57"/>
       <c r="E49" s="57"/>
@@ -15746,10 +16464,11 @@
       <c r="Z49" s="57"/>
       <c r="AA49" s="57"/>
       <c r="AB49" s="57"/>
-    </row>
-    <row r="50" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="54"/>
-      <c r="B50" s="55"/>
+      <c r="AC49" s="57"/>
+    </row>
+    <row r="50" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="58"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="55"/>
       <c r="D50" s="55"/>
       <c r="E50" s="55"/>
@@ -15776,10 +16495,11 @@
       <c r="Z50" s="55"/>
       <c r="AA50" s="55"/>
       <c r="AB50" s="55"/>
-    </row>
-    <row r="51" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="56"/>
-      <c r="B51" s="57"/>
+      <c r="AC50" s="55"/>
+    </row>
+    <row r="51" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="58"/>
+      <c r="B51" s="56"/>
       <c r="C51" s="57"/>
       <c r="D51" s="57"/>
       <c r="E51" s="57"/>
@@ -15806,10 +16526,11 @@
       <c r="Z51" s="57"/>
       <c r="AA51" s="57"/>
       <c r="AB51" s="57"/>
-    </row>
-    <row r="52" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="54"/>
-      <c r="B52" s="55"/>
+      <c r="AC51" s="57"/>
+    </row>
+    <row r="52" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="58"/>
+      <c r="B52" s="54"/>
       <c r="C52" s="55"/>
       <c r="D52" s="55"/>
       <c r="E52" s="55"/>
@@ -15836,10 +16557,11 @@
       <c r="Z52" s="55"/>
       <c r="AA52" s="55"/>
       <c r="AB52" s="55"/>
-    </row>
-    <row r="53" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="56"/>
-      <c r="B53" s="57"/>
+      <c r="AC52" s="55"/>
+    </row>
+    <row r="53" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="58"/>
+      <c r="B53" s="56"/>
       <c r="C53" s="57"/>
       <c r="D53" s="57"/>
       <c r="E53" s="57"/>
@@ -15866,10 +16588,11 @@
       <c r="Z53" s="57"/>
       <c r="AA53" s="57"/>
       <c r="AB53" s="57"/>
-    </row>
-    <row r="54" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="54"/>
-      <c r="B54" s="55"/>
+      <c r="AC53" s="57"/>
+    </row>
+    <row r="54" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="58"/>
+      <c r="B54" s="54"/>
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
       <c r="E54" s="55"/>
@@ -15896,10 +16619,11 @@
       <c r="Z54" s="55"/>
       <c r="AA54" s="55"/>
       <c r="AB54" s="55"/>
-    </row>
-    <row r="55" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="56"/>
-      <c r="B55" s="57"/>
+      <c r="AC54" s="55"/>
+    </row>
+    <row r="55" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="58"/>
+      <c r="B55" s="56"/>
       <c r="C55" s="57"/>
       <c r="D55" s="57"/>
       <c r="E55" s="57"/>
@@ -15926,10 +16650,11 @@
       <c r="Z55" s="57"/>
       <c r="AA55" s="57"/>
       <c r="AB55" s="57"/>
-    </row>
-    <row r="56" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="54"/>
-      <c r="B56" s="55"/>
+      <c r="AC55" s="57"/>
+    </row>
+    <row r="56" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="58"/>
+      <c r="B56" s="54"/>
       <c r="C56" s="55"/>
       <c r="D56" s="55"/>
       <c r="E56" s="55"/>
@@ -15956,10 +16681,11 @@
       <c r="Z56" s="55"/>
       <c r="AA56" s="55"/>
       <c r="AB56" s="55"/>
-    </row>
-    <row r="57" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="56"/>
-      <c r="B57" s="57"/>
+      <c r="AC56" s="55"/>
+    </row>
+    <row r="57" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="58"/>
+      <c r="B57" s="56"/>
       <c r="C57" s="57"/>
       <c r="D57" s="57"/>
       <c r="E57" s="57"/>
@@ -15986,10 +16712,11 @@
       <c r="Z57" s="57"/>
       <c r="AA57" s="57"/>
       <c r="AB57" s="57"/>
-    </row>
-    <row r="58" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="54"/>
-      <c r="B58" s="55"/>
+      <c r="AC57" s="57"/>
+    </row>
+    <row r="58" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="58"/>
+      <c r="B58" s="54"/>
       <c r="C58" s="55"/>
       <c r="D58" s="55"/>
       <c r="E58" s="55"/>
@@ -16016,10 +16743,11 @@
       <c r="Z58" s="55"/>
       <c r="AA58" s="55"/>
       <c r="AB58" s="55"/>
-    </row>
-    <row r="59" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="56"/>
-      <c r="B59" s="57"/>
+      <c r="AC58" s="55"/>
+    </row>
+    <row r="59" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="58"/>
+      <c r="B59" s="56"/>
       <c r="C59" s="57"/>
       <c r="D59" s="57"/>
       <c r="E59" s="57"/>
@@ -16046,10 +16774,11 @@
       <c r="Z59" s="57"/>
       <c r="AA59" s="57"/>
       <c r="AB59" s="57"/>
-    </row>
-    <row r="60" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="54"/>
-      <c r="B60" s="55"/>
+      <c r="AC59" s="57"/>
+    </row>
+    <row r="60" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="58"/>
+      <c r="B60" s="54"/>
       <c r="C60" s="55"/>
       <c r="D60" s="55"/>
       <c r="E60" s="55"/>
@@ -16076,10 +16805,11 @@
       <c r="Z60" s="55"/>
       <c r="AA60" s="55"/>
       <c r="AB60" s="55"/>
-    </row>
-    <row r="61" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="56"/>
-      <c r="B61" s="57"/>
+      <c r="AC60" s="55"/>
+    </row>
+    <row r="61" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="58"/>
+      <c r="B61" s="56"/>
       <c r="C61" s="57"/>
       <c r="D61" s="57"/>
       <c r="E61" s="57"/>
@@ -16106,6 +16836,108 @@
       <c r="Z61" s="57"/>
       <c r="AA61" s="57"/>
       <c r="AB61" s="57"/>
+      <c r="AC61" s="57"/>
+    </row>
+    <row r="62" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="58"/>
+      <c r="B62" s="54"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="55"/>
+      <c r="J62" s="55"/>
+      <c r="K62" s="55"/>
+      <c r="L62" s="55"/>
+      <c r="M62" s="55"/>
+      <c r="N62" s="55"/>
+      <c r="O62" s="55"/>
+      <c r="P62" s="55"/>
+      <c r="Q62" s="55"/>
+      <c r="R62" s="55"/>
+      <c r="S62" s="55"/>
+      <c r="T62" s="55"/>
+      <c r="U62" s="55"/>
+      <c r="V62" s="55"/>
+      <c r="W62" s="55"/>
+      <c r="X62" s="55"/>
+      <c r="Y62" s="55"/>
+      <c r="Z62" s="55"/>
+      <c r="AA62" s="55"/>
+      <c r="AB62" s="55"/>
+      <c r="AC62" s="55"/>
+    </row>
+    <row r="63" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="58"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="57"/>
+      <c r="F63" s="57"/>
+      <c r="G63" s="57"/>
+      <c r="H63" s="57"/>
+      <c r="I63" s="57"/>
+      <c r="J63" s="57"/>
+      <c r="K63" s="57"/>
+      <c r="L63" s="57"/>
+      <c r="M63" s="57"/>
+      <c r="N63" s="57"/>
+      <c r="O63" s="57"/>
+      <c r="P63" s="57"/>
+      <c r="Q63" s="57"/>
+      <c r="R63" s="57"/>
+      <c r="S63" s="57"/>
+      <c r="T63" s="57"/>
+      <c r="U63" s="57"/>
+      <c r="V63" s="57"/>
+      <c r="W63" s="57"/>
+      <c r="X63" s="57"/>
+      <c r="Y63" s="57"/>
+      <c r="Z63" s="57"/>
+      <c r="AA63" s="57"/>
+      <c r="AB63" s="57"/>
+      <c r="AC63" s="57"/>
+    </row>
+    <row r="64" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="58"/>
+      <c r="B64" s="54"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="55"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="55"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="55"/>
+      <c r="I64" s="55"/>
+      <c r="J64" s="55"/>
+      <c r="K64" s="55"/>
+      <c r="L64" s="55"/>
+      <c r="M64" s="55"/>
+      <c r="N64" s="55"/>
+      <c r="O64" s="55"/>
+      <c r="P64" s="55"/>
+      <c r="Q64" s="55"/>
+      <c r="R64" s="55"/>
+      <c r="S64" s="55"/>
+      <c r="T64" s="55"/>
+      <c r="U64" s="55"/>
+      <c r="V64" s="55"/>
+      <c r="W64" s="55"/>
+      <c r="X64" s="55"/>
+      <c r="Y64" s="55"/>
+      <c r="Z64" s="55"/>
+      <c r="AA64" s="55"/>
+      <c r="AB64" s="55"/>
+      <c r="AC64" s="55"/>
+    </row>
+    <row r="65" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U65" s="48"/>
+      <c r="V65" s="18"/>
+    </row>
+    <row r="66" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U66" s="48"/>
+      <c r="V66" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>